<commit_message>
Run Match button rearranged to the level of filenames
</commit_message>
<xml_diff>
--- a/Resources/Steel-Pole/Steel Book POLE_MATCHED.xlsx
+++ b/Resources/Steel-Pole/Steel Book POLE_MATCHED.xlsx
@@ -965,301 +965,324 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr"/>
-      <c r="B17" s="2" t="inlineStr"/>
-      <c r="C17" s="6" t="inlineStr">
+      <c r="A17" s="20" t="inlineStr">
+        <is>
+          <t>M126</t>
+        </is>
+      </c>
+      <c r="B17" s="21" t="inlineStr"/>
+      <c r="C17" s="22" t="inlineStr">
         <is>
           <t>01/Jun/2025</t>
         </is>
       </c>
-      <c r="D17" s="1" t="inlineStr">
+      <c r="D17" s="20" t="inlineStr">
         <is>
           <t>Dr</t>
         </is>
       </c>
-      <c r="E17" s="7" t="inlineStr">
+      <c r="E17" s="23" t="inlineStr">
         <is>
           <t>Mutual Trust Bank Ltd-SND-002-0320004355</t>
         </is>
       </c>
-      <c r="F17" s="1" t="inlineStr"/>
-      <c r="G17" s="1" t="inlineStr"/>
-      <c r="H17" s="9" t="inlineStr">
+      <c r="F17" s="20" t="inlineStr"/>
+      <c r="G17" s="20" t="inlineStr"/>
+      <c r="H17" s="24" t="inlineStr">
         <is>
           <t>Receipt</t>
         </is>
       </c>
-      <c r="I17" s="1" t="inlineStr">
+      <c r="I17" s="20" t="inlineStr">
         <is>
           <t>915</t>
         </is>
       </c>
-      <c r="J17" s="1" t="inlineStr"/>
-      <c r="K17" s="8" t="inlineStr">
+      <c r="J17" s="20" t="inlineStr"/>
+      <c r="K17" s="25" t="inlineStr">
         <is>
           <t>905515</t>
         </is>
       </c>
-      <c r="L17" s="1" t="inlineStr"/>
+      <c r="L17" s="20" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr"/>
-      <c r="B18" s="2" t="inlineStr">
-        <is>
-          <t>Unmatched Record
-Reasons:
-1. No interunit account found in File 2 block
-2. Settlement mismatch: File 1 IDs ['94976'], File 2 IDs []</t>
-        </is>
-      </c>
-      <c r="C18" s="1" t="inlineStr"/>
-      <c r="D18" s="1" t="inlineStr"/>
-      <c r="E18" s="10" t="inlineStr">
+      <c r="A18" s="20" t="inlineStr">
+        <is>
+          <t>M126</t>
+        </is>
+      </c>
+      <c r="B18" s="21" t="inlineStr">
+        <is>
+          <t>Manual Match
+Lender Amount: 905515.00
+Borrower Amount: 905515.00</t>
+        </is>
+      </c>
+      <c r="C18" s="20" t="inlineStr"/>
+      <c r="D18" s="20" t="inlineStr"/>
+      <c r="E18" s="26" t="inlineStr">
         <is>
           <t>Reversing....     Bank Payment date was 26.12.2024</t>
         </is>
       </c>
-      <c r="F18" s="1" t="inlineStr"/>
-      <c r="G18" s="1" t="inlineStr"/>
-      <c r="H18" s="1" t="inlineStr"/>
-      <c r="I18" s="1" t="inlineStr"/>
-      <c r="J18" s="1" t="inlineStr"/>
-      <c r="K18" s="1" t="inlineStr"/>
-      <c r="L18" s="1" t="inlineStr"/>
+      <c r="F18" s="20" t="inlineStr"/>
+      <c r="G18" s="20" t="inlineStr"/>
+      <c r="H18" s="20" t="inlineStr"/>
+      <c r="I18" s="20" t="inlineStr"/>
+      <c r="J18" s="20" t="inlineStr"/>
+      <c r="K18" s="20" t="inlineStr"/>
+      <c r="L18" s="20" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr"/>
-      <c r="B19" s="2" t="inlineStr"/>
-      <c r="C19" s="1" t="inlineStr"/>
-      <c r="D19" s="1" t="inlineStr">
+      <c r="A19" s="20" t="inlineStr">
+        <is>
+          <t>M126</t>
+        </is>
+      </c>
+      <c r="B19" s="21" t="inlineStr"/>
+      <c r="C19" s="20" t="inlineStr"/>
+      <c r="D19" s="20" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E19" s="11" t="inlineStr">
+      <c r="E19" s="27" t="inlineStr">
         <is>
           <t>g.azam</t>
         </is>
       </c>
-      <c r="F19" s="1" t="inlineStr"/>
-      <c r="G19" s="1" t="inlineStr"/>
-      <c r="H19" s="1" t="inlineStr"/>
-      <c r="I19" s="1" t="inlineStr"/>
-      <c r="J19" s="1" t="inlineStr"/>
-      <c r="K19" s="1" t="inlineStr"/>
-      <c r="L19" s="1" t="inlineStr"/>
+      <c r="F19" s="20" t="inlineStr"/>
+      <c r="G19" s="20" t="inlineStr"/>
+      <c r="H19" s="20" t="inlineStr"/>
+      <c r="I19" s="20" t="inlineStr"/>
+      <c r="J19" s="20" t="inlineStr"/>
+      <c r="K19" s="20" t="inlineStr"/>
+      <c r="L19" s="20" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="20" t="inlineStr">
+      <c r="A20" s="12" t="inlineStr">
         <is>
           <t>M122</t>
         </is>
       </c>
-      <c r="B20" s="21" t="inlineStr"/>
-      <c r="C20" s="22" t="inlineStr">
+      <c r="B20" s="13" t="inlineStr"/>
+      <c r="C20" s="14" t="inlineStr">
         <is>
           <t>02/Jun/2025</t>
         </is>
       </c>
-      <c r="D20" s="20" t="inlineStr">
+      <c r="D20" s="12" t="inlineStr">
         <is>
           <t>Dr</t>
         </is>
       </c>
-      <c r="E20" s="23" t="inlineStr">
+      <c r="E20" s="15" t="inlineStr">
         <is>
           <t>Eastern Bank PLC-OD-A/C-1012040000125</t>
         </is>
       </c>
-      <c r="F20" s="20" t="inlineStr"/>
-      <c r="G20" s="20" t="inlineStr"/>
-      <c r="H20" s="24" t="inlineStr">
+      <c r="F20" s="12" t="inlineStr"/>
+      <c r="G20" s="12" t="inlineStr"/>
+      <c r="H20" s="16" t="inlineStr">
         <is>
           <t>Receipt</t>
         </is>
       </c>
-      <c r="I20" s="20" t="inlineStr">
+      <c r="I20" s="12" t="inlineStr">
         <is>
           <t>927</t>
         </is>
       </c>
-      <c r="J20" s="20" t="inlineStr"/>
-      <c r="K20" s="25" t="inlineStr">
+      <c r="J20" s="12" t="inlineStr"/>
+      <c r="K20" s="17" t="inlineStr">
         <is>
           <t>18027176.54</t>
         </is>
       </c>
-      <c r="L20" s="20" t="inlineStr">
+      <c r="L20" s="12" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="20" t="inlineStr">
+      <c r="A21" s="12" t="inlineStr">
         <is>
           <t>M122</t>
         </is>
       </c>
-      <c r="B21" s="21" t="inlineStr">
+      <c r="B21" s="13" t="inlineStr">
         <is>
           <t>USD Match: $147,401.28
 Lender Amount: 18027176.54
 Borrower Amount: 18027176.54</t>
         </is>
       </c>
-      <c r="C21" s="20" t="inlineStr"/>
-      <c r="D21" s="20" t="inlineStr"/>
-      <c r="E21" s="26" t="inlineStr">
+      <c r="C21" s="12" t="inlineStr"/>
+      <c r="D21" s="12" t="inlineStr"/>
+      <c r="E21" s="18" t="inlineStr">
         <is>
           <t>Received Voucher: Amounts received agt PO number : MCEP/BREB/DMD-SPC-G-24-Lot-1/2023-2024-Part-1-WB, remark: Total Bill- 226851.20 usd. CIL Bill- Part1- 193819.20 usd+ Part2- 33032 usd) Total received- 226771.20 (Part1- 193819.20 usd+ Part2- 32952 usd). Bank charge -80 Usd.,  $147,401.28 @ Tk.122.30/-</t>
         </is>
       </c>
-      <c r="F21" s="20" t="inlineStr"/>
-      <c r="G21" s="20" t="inlineStr"/>
-      <c r="H21" s="20" t="inlineStr"/>
-      <c r="I21" s="20" t="inlineStr"/>
-      <c r="J21" s="20" t="inlineStr"/>
-      <c r="K21" s="20" t="inlineStr"/>
-      <c r="L21" s="20" t="inlineStr">
+      <c r="F21" s="12" t="inlineStr"/>
+      <c r="G21" s="12" t="inlineStr"/>
+      <c r="H21" s="12" t="inlineStr"/>
+      <c r="I21" s="12" t="inlineStr"/>
+      <c r="J21" s="12" t="inlineStr"/>
+      <c r="K21" s="12" t="inlineStr"/>
+      <c r="L21" s="12" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="20" t="inlineStr">
+      <c r="A22" s="12" t="inlineStr">
         <is>
           <t>M122</t>
         </is>
       </c>
-      <c r="B22" s="21" t="inlineStr"/>
-      <c r="C22" s="20" t="inlineStr"/>
-      <c r="D22" s="20" t="inlineStr">
+      <c r="B22" s="13" t="inlineStr"/>
+      <c r="C22" s="12" t="inlineStr"/>
+      <c r="D22" s="12" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E22" s="27" t="inlineStr">
+      <c r="E22" s="19" t="inlineStr">
         <is>
           <t>ashiq</t>
         </is>
       </c>
-      <c r="F22" s="20" t="inlineStr"/>
-      <c r="G22" s="20" t="inlineStr"/>
-      <c r="H22" s="20" t="inlineStr"/>
-      <c r="I22" s="20" t="inlineStr"/>
-      <c r="J22" s="20" t="inlineStr"/>
-      <c r="K22" s="20" t="inlineStr"/>
-      <c r="L22" s="20" t="inlineStr">
+      <c r="F22" s="12" t="inlineStr"/>
+      <c r="G22" s="12" t="inlineStr"/>
+      <c r="H22" s="12" t="inlineStr"/>
+      <c r="I22" s="12" t="inlineStr"/>
+      <c r="J22" s="12" t="inlineStr"/>
+      <c r="K22" s="12" t="inlineStr"/>
+      <c r="L22" s="12" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="12" t="inlineStr">
+      <c r="A23" s="20" t="inlineStr">
         <is>
           <t>M073</t>
         </is>
       </c>
-      <c r="B23" s="13" t="inlineStr"/>
-      <c r="C23" s="14" t="inlineStr">
+      <c r="B23" s="21" t="inlineStr"/>
+      <c r="C23" s="22" t="inlineStr">
         <is>
           <t>03/Jun/2025</t>
         </is>
       </c>
-      <c r="D23" s="12" t="inlineStr">
+      <c r="D23" s="20" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E23" s="15" t="inlineStr">
+      <c r="E23" s="23" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F23" s="12" t="inlineStr"/>
-      <c r="G23" s="12" t="inlineStr"/>
-      <c r="H23" s="16" t="inlineStr">
+      <c r="F23" s="20" t="inlineStr"/>
+      <c r="G23" s="20" t="inlineStr"/>
+      <c r="H23" s="24" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I23" s="12" t="inlineStr">
+      <c r="I23" s="20" t="inlineStr">
         <is>
           <t>70391</t>
         </is>
       </c>
-      <c r="J23" s="17" t="inlineStr">
+      <c r="J23" s="25" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="K23" s="12" t="inlineStr"/>
-      <c r="L23" s="12" t="inlineStr">
+      <c r="K23" s="20" t="inlineStr"/>
+      <c r="L23" s="20" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="12" t="inlineStr">
+      <c r="A24" s="20" t="inlineStr">
         <is>
           <t>M073</t>
         </is>
       </c>
-      <c r="B24" s="13" t="inlineStr">
+      <c r="B24" s="21" t="inlineStr">
         <is>
           <t>Interunit Loan Match: MDB#0331
 Lender Amount: 600000.00
 Borrower Amount: 600000.00</t>
         </is>
       </c>
-      <c r="C24" s="12" t="inlineStr"/>
-      <c r="D24" s="12" t="inlineStr"/>
-      <c r="E24" s="18" t="inlineStr">
+      <c r="C24" s="20" t="inlineStr"/>
+      <c r="D24" s="20" t="inlineStr"/>
+      <c r="E24" s="26" t="inlineStr">
         <is>
           <t>Being the amount paid to M/S. Mukta Engineering Works . Supply of , Invoice Number:  005, Challan Number: 005, Work Order Number: PBS/PO/2024/8/29211, BA Team (A), Company Unit: Concrete Pole &amp; Pile, Project Name : PBSF-G-260 (ID:949763), Work Order date: 2024-08-30, Goods Received Date: 2024-12-04, Work Order Value: 853990.0, Total Bill Amount: 797190.0, TDS Deduction Amount: 0.0, VDS Deduction Amount: 0.0</t>
         </is>
       </c>
-      <c r="F24" s="12" t="inlineStr"/>
-      <c r="G24" s="12" t="inlineStr"/>
-      <c r="H24" s="12" t="inlineStr"/>
-      <c r="I24" s="12" t="inlineStr"/>
-      <c r="J24" s="12" t="inlineStr"/>
-      <c r="K24" s="12" t="inlineStr"/>
-      <c r="L24" s="12" t="inlineStr">
+      <c r="F24" s="20" t="inlineStr"/>
+      <c r="G24" s="20" t="inlineStr"/>
+      <c r="H24" s="20" t="inlineStr"/>
+      <c r="I24" s="20" t="inlineStr"/>
+      <c r="J24" s="20" t="inlineStr"/>
+      <c r="K24" s="20" t="inlineStr"/>
+      <c r="L24" s="20" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="12" t="inlineStr">
+      <c r="A25" s="20" t="inlineStr">
         <is>
           <t>M073</t>
         </is>
       </c>
-      <c r="B25" s="13" t="inlineStr"/>
-      <c r="C25" s="12" t="inlineStr"/>
-      <c r="D25" s="12" t="inlineStr">
+      <c r="B25" s="21" t="inlineStr"/>
+      <c r="C25" s="20" t="inlineStr"/>
+      <c r="D25" s="20" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E25" s="19" t="inlineStr">
+      <c r="E25" s="27" t="inlineStr">
         <is>
           <t>ziaul</t>
         </is>
       </c>
-      <c r="F25" s="12" t="inlineStr"/>
-      <c r="G25" s="12" t="inlineStr"/>
-      <c r="H25" s="12" t="inlineStr"/>
-      <c r="I25" s="12" t="inlineStr"/>
-      <c r="J25" s="12" t="inlineStr"/>
-      <c r="K25" s="12" t="inlineStr"/>
-      <c r="L25" s="12" t="inlineStr">
+      <c r="F25" s="20" t="inlineStr"/>
+      <c r="G25" s="20" t="inlineStr"/>
+      <c r="H25" s="20" t="inlineStr"/>
+      <c r="I25" s="20" t="inlineStr"/>
+      <c r="J25" s="20" t="inlineStr"/>
+      <c r="K25" s="20" t="inlineStr"/>
+      <c r="L25" s="20" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
@@ -1440,433 +1463,433 @@
       <c r="L28" s="1" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" s="20" t="inlineStr">
+      <c r="A29" s="12" t="inlineStr">
         <is>
           <t>M077</t>
         </is>
       </c>
-      <c r="B29" s="21" t="inlineStr"/>
-      <c r="C29" s="22" t="inlineStr">
+      <c r="B29" s="13" t="inlineStr"/>
+      <c r="C29" s="14" t="inlineStr">
         <is>
           <t>03/Jun/2025</t>
         </is>
       </c>
-      <c r="D29" s="20" t="inlineStr">
+      <c r="D29" s="12" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E29" s="23" t="inlineStr">
+      <c r="E29" s="15" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F29" s="20" t="inlineStr"/>
-      <c r="G29" s="20" t="inlineStr"/>
-      <c r="H29" s="24" t="inlineStr">
+      <c r="F29" s="12" t="inlineStr"/>
+      <c r="G29" s="12" t="inlineStr"/>
+      <c r="H29" s="16" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I29" s="20" t="inlineStr">
+      <c r="I29" s="12" t="inlineStr">
         <is>
           <t>70394</t>
         </is>
       </c>
-      <c r="J29" s="25" t="inlineStr">
+      <c r="J29" s="17" t="inlineStr">
         <is>
           <t>700000</t>
         </is>
       </c>
-      <c r="K29" s="20" t="inlineStr"/>
-      <c r="L29" s="20" t="inlineStr">
+      <c r="K29" s="12" t="inlineStr"/>
+      <c r="L29" s="12" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="20" t="inlineStr">
+      <c r="A30" s="12" t="inlineStr">
         <is>
           <t>M077</t>
         </is>
       </c>
-      <c r="B30" s="21" t="inlineStr">
+      <c r="B30" s="13" t="inlineStr">
         <is>
           <t>Interunit Loan Match: MDB#0331
 Lender Amount: 700000.00
 Borrower Amount: 700000.00</t>
         </is>
       </c>
-      <c r="C30" s="20" t="inlineStr"/>
-      <c r="D30" s="20" t="inlineStr"/>
-      <c r="E30" s="26" t="inlineStr">
+      <c r="C30" s="12" t="inlineStr"/>
+      <c r="D30" s="12" t="inlineStr"/>
+      <c r="E30" s="18" t="inlineStr">
         <is>
           <t>Being the amount paid to Akij Cement Company Ltd.. Supply of , Invoice Number:  NOV24-14 (Bag), Challan Number: DC01020247652,DC01020246583, DC01020246584,DC01020247653, DC01020247654, Work Order Number: G24/PO/2024/9/29253, BA Team (A), Company Unit: Concrete Pole &amp; Pile, Project Name : WD1: LOT-1; MCEP/BREB/DMD SPC-G-24, Lot-1, Work Order date: 2024-09-03, Goods Received Date: 2024-11-05, Work Order Value: 5400000.0, Total Bill Amount: 873603.36, TDS Deduction Amount: 17828.64, VDS Deduction Amount: 0.0</t>
         </is>
       </c>
-      <c r="F30" s="20" t="inlineStr"/>
-      <c r="G30" s="20" t="inlineStr"/>
-      <c r="H30" s="20" t="inlineStr"/>
-      <c r="I30" s="20" t="inlineStr"/>
-      <c r="J30" s="20" t="inlineStr"/>
-      <c r="K30" s="20" t="inlineStr"/>
-      <c r="L30" s="20" t="inlineStr">
+      <c r="F30" s="12" t="inlineStr"/>
+      <c r="G30" s="12" t="inlineStr"/>
+      <c r="H30" s="12" t="inlineStr"/>
+      <c r="I30" s="12" t="inlineStr"/>
+      <c r="J30" s="12" t="inlineStr"/>
+      <c r="K30" s="12" t="inlineStr"/>
+      <c r="L30" s="12" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="20" t="inlineStr">
+      <c r="A31" s="12" t="inlineStr">
         <is>
           <t>M077</t>
         </is>
       </c>
-      <c r="B31" s="21" t="inlineStr"/>
-      <c r="C31" s="20" t="inlineStr"/>
-      <c r="D31" s="20" t="inlineStr">
+      <c r="B31" s="13" t="inlineStr"/>
+      <c r="C31" s="12" t="inlineStr"/>
+      <c r="D31" s="12" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E31" s="27" t="inlineStr">
+      <c r="E31" s="19" t="inlineStr">
         <is>
           <t>ziaul</t>
         </is>
       </c>
-      <c r="F31" s="20" t="inlineStr"/>
-      <c r="G31" s="20" t="inlineStr"/>
-      <c r="H31" s="20" t="inlineStr"/>
-      <c r="I31" s="20" t="inlineStr"/>
-      <c r="J31" s="20" t="inlineStr"/>
-      <c r="K31" s="20" t="inlineStr"/>
-      <c r="L31" s="20" t="inlineStr">
+      <c r="F31" s="12" t="inlineStr"/>
+      <c r="G31" s="12" t="inlineStr"/>
+      <c r="H31" s="12" t="inlineStr"/>
+      <c r="I31" s="12" t="inlineStr"/>
+      <c r="J31" s="12" t="inlineStr"/>
+      <c r="K31" s="12" t="inlineStr"/>
+      <c r="L31" s="12" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="12" t="inlineStr">
+      <c r="A32" s="20" t="inlineStr">
         <is>
           <t>M001</t>
         </is>
       </c>
-      <c r="B32" s="13" t="inlineStr"/>
-      <c r="C32" s="14" t="inlineStr">
+      <c r="B32" s="21" t="inlineStr"/>
+      <c r="C32" s="22" t="inlineStr">
         <is>
           <t>03/Jun/2025</t>
         </is>
       </c>
-      <c r="D32" s="12" t="inlineStr">
+      <c r="D32" s="20" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E32" s="15" t="inlineStr">
+      <c r="E32" s="23" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F32" s="12" t="inlineStr"/>
-      <c r="G32" s="12" t="inlineStr"/>
-      <c r="H32" s="16" t="inlineStr">
+      <c r="F32" s="20" t="inlineStr"/>
+      <c r="G32" s="20" t="inlineStr"/>
+      <c r="H32" s="24" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I32" s="12" t="inlineStr">
+      <c r="I32" s="20" t="inlineStr">
         <is>
           <t>70395</t>
         </is>
       </c>
-      <c r="J32" s="17" t="inlineStr">
+      <c r="J32" s="25" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="K32" s="12" t="inlineStr"/>
-      <c r="L32" s="12" t="inlineStr">
+      <c r="K32" s="20" t="inlineStr"/>
+      <c r="L32" s="20" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="12" t="inlineStr">
+      <c r="A33" s="20" t="inlineStr">
         <is>
           <t>M001</t>
         </is>
       </c>
-      <c r="B33" s="13" t="inlineStr">
+      <c r="B33" s="21" t="inlineStr">
         <is>
           <t>PO Match: DMD/PO/2024/12/31413
 Lender Amount: 300000.00
 Borrower Amount: 300000.00</t>
         </is>
       </c>
-      <c r="C33" s="12" t="inlineStr"/>
-      <c r="D33" s="12" t="inlineStr"/>
-      <c r="E33" s="18" t="inlineStr">
+      <c r="C33" s="20" t="inlineStr"/>
+      <c r="D33" s="20" t="inlineStr"/>
+      <c r="E33" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve">Being the amount paid to M/S. Alif  Enterprise. Supply of , Invoice Number:  214, Challan Number: 011,012,013,015,005,007,008,009,010.,014, 016, 017,020, Work Order Number: DMD/PO/2024/12/31413, BA Team (A), Company Unit: Concrete Pole &amp; Pile, Project Name : DMD-SPC-G-24-Lot-1-Part-2-WB, Work Order date: 2024-12-30, Goods Received Date: 2025-01-18,2025-01-11,2025-01-30, Work Order Value: 1104000.0, Total Bill Amount: 300000.0, TDS Deduction Amount: 0.0, VDS Deduction Amount: 0.0  P-58272_x000D_
 </t>
         </is>
       </c>
-      <c r="F33" s="12" t="inlineStr"/>
-      <c r="G33" s="12" t="inlineStr"/>
-      <c r="H33" s="12" t="inlineStr"/>
-      <c r="I33" s="12" t="inlineStr"/>
-      <c r="J33" s="12" t="inlineStr"/>
-      <c r="K33" s="12" t="inlineStr"/>
-      <c r="L33" s="12" t="inlineStr">
+      <c r="F33" s="20" t="inlineStr"/>
+      <c r="G33" s="20" t="inlineStr"/>
+      <c r="H33" s="20" t="inlineStr"/>
+      <c r="I33" s="20" t="inlineStr"/>
+      <c r="J33" s="20" t="inlineStr"/>
+      <c r="K33" s="20" t="inlineStr"/>
+      <c r="L33" s="20" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="12" t="inlineStr">
+      <c r="A34" s="20" t="inlineStr">
         <is>
           <t>M001</t>
         </is>
       </c>
-      <c r="B34" s="13" t="inlineStr"/>
-      <c r="C34" s="12" t="inlineStr"/>
-      <c r="D34" s="12" t="inlineStr">
+      <c r="B34" s="21" t="inlineStr"/>
+      <c r="C34" s="20" t="inlineStr"/>
+      <c r="D34" s="20" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E34" s="19" t="inlineStr">
+      <c r="E34" s="27" t="inlineStr">
         <is>
           <t>mahbub.alam</t>
         </is>
       </c>
-      <c r="F34" s="12" t="inlineStr"/>
-      <c r="G34" s="12" t="inlineStr"/>
-      <c r="H34" s="12" t="inlineStr"/>
-      <c r="I34" s="12" t="inlineStr"/>
-      <c r="J34" s="12" t="inlineStr"/>
-      <c r="K34" s="12" t="inlineStr"/>
-      <c r="L34" s="12" t="inlineStr">
+      <c r="F34" s="20" t="inlineStr"/>
+      <c r="G34" s="20" t="inlineStr"/>
+      <c r="H34" s="20" t="inlineStr"/>
+      <c r="I34" s="20" t="inlineStr"/>
+      <c r="J34" s="20" t="inlineStr"/>
+      <c r="K34" s="20" t="inlineStr"/>
+      <c r="L34" s="20" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="20" t="inlineStr">
+      <c r="A35" s="12" t="inlineStr">
         <is>
           <t>M075</t>
         </is>
       </c>
-      <c r="B35" s="21" t="inlineStr"/>
-      <c r="C35" s="22" t="inlineStr">
+      <c r="B35" s="13" t="inlineStr"/>
+      <c r="C35" s="14" t="inlineStr">
         <is>
           <t>03/Jun/2025</t>
         </is>
       </c>
-      <c r="D35" s="20" t="inlineStr">
+      <c r="D35" s="12" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E35" s="23" t="inlineStr">
+      <c r="E35" s="15" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F35" s="20" t="inlineStr"/>
-      <c r="G35" s="20" t="inlineStr"/>
-      <c r="H35" s="24" t="inlineStr">
+      <c r="F35" s="12" t="inlineStr"/>
+      <c r="G35" s="12" t="inlineStr"/>
+      <c r="H35" s="16" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I35" s="20" t="inlineStr">
+      <c r="I35" s="12" t="inlineStr">
         <is>
           <t>70396</t>
         </is>
       </c>
-      <c r="J35" s="25" t="inlineStr">
+      <c r="J35" s="17" t="inlineStr">
         <is>
           <t>700000</t>
         </is>
       </c>
-      <c r="K35" s="20" t="inlineStr"/>
-      <c r="L35" s="20" t="inlineStr">
+      <c r="K35" s="12" t="inlineStr"/>
+      <c r="L35" s="12" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="20" t="inlineStr">
+      <c r="A36" s="12" t="inlineStr">
         <is>
           <t>M075</t>
         </is>
       </c>
-      <c r="B36" s="21" t="inlineStr">
+      <c r="B36" s="13" t="inlineStr">
         <is>
           <t>Interunit Loan Match: MDB#0331
 Lender Amount: 700000.00
 Borrower Amount: 700000.00</t>
         </is>
       </c>
-      <c r="C36" s="20" t="inlineStr"/>
-      <c r="D36" s="20" t="inlineStr"/>
-      <c r="E36" s="26" t="inlineStr">
+      <c r="C36" s="12" t="inlineStr"/>
+      <c r="D36" s="12" t="inlineStr"/>
+      <c r="E36" s="18" t="inlineStr">
         <is>
           <t>Being the amount paid to Crown Cement PLC. Supply of , Invoice Number:  147, Challan Number: 8002103646, 8002103650,8002107843, 8002107850,8002103872, 8002103674,8002112659, 8002112833, 8002112835, 8002112911, 8002112961,,8002116901, 8002116920,8002121931,8002107848, Work Order Number: PBS/PO/2024/11/30298, BA Team (A), Company Unit: Concrete Pole &amp; Pile, Project Name : PBSF-G-260 (ID:949763), Work Order date: 2024-11-07, Goods Received Date: 2024-11-21,2024-11-28,2024-12-05,2024-12-02, Work Order Value: 3120000.0, Total Bill Amount: 2777895.84, TDS Deduction Amount: 56691.75, VDS Deduction Amount: 0.0</t>
         </is>
       </c>
-      <c r="F36" s="20" t="inlineStr"/>
-      <c r="G36" s="20" t="inlineStr"/>
-      <c r="H36" s="20" t="inlineStr"/>
-      <c r="I36" s="20" t="inlineStr"/>
-      <c r="J36" s="20" t="inlineStr"/>
-      <c r="K36" s="20" t="inlineStr"/>
-      <c r="L36" s="20" t="inlineStr">
+      <c r="F36" s="12" t="inlineStr"/>
+      <c r="G36" s="12" t="inlineStr"/>
+      <c r="H36" s="12" t="inlineStr"/>
+      <c r="I36" s="12" t="inlineStr"/>
+      <c r="J36" s="12" t="inlineStr"/>
+      <c r="K36" s="12" t="inlineStr"/>
+      <c r="L36" s="12" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="20" t="inlineStr">
+      <c r="A37" s="12" t="inlineStr">
         <is>
           <t>M075</t>
         </is>
       </c>
-      <c r="B37" s="21" t="inlineStr"/>
-      <c r="C37" s="20" t="inlineStr"/>
-      <c r="D37" s="20" t="inlineStr">
+      <c r="B37" s="13" t="inlineStr"/>
+      <c r="C37" s="12" t="inlineStr"/>
+      <c r="D37" s="12" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E37" s="27" t="inlineStr">
+      <c r="E37" s="19" t="inlineStr">
         <is>
           <t>ziaul</t>
         </is>
       </c>
-      <c r="F37" s="20" t="inlineStr"/>
-      <c r="G37" s="20" t="inlineStr"/>
-      <c r="H37" s="20" t="inlineStr"/>
-      <c r="I37" s="20" t="inlineStr"/>
-      <c r="J37" s="20" t="inlineStr"/>
-      <c r="K37" s="20" t="inlineStr"/>
-      <c r="L37" s="20" t="inlineStr">
+      <c r="F37" s="12" t="inlineStr"/>
+      <c r="G37" s="12" t="inlineStr"/>
+      <c r="H37" s="12" t="inlineStr"/>
+      <c r="I37" s="12" t="inlineStr"/>
+      <c r="J37" s="12" t="inlineStr"/>
+      <c r="K37" s="12" t="inlineStr"/>
+      <c r="L37" s="12" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="12" t="inlineStr">
+      <c r="A38" s="20" t="inlineStr">
         <is>
           <t>M076</t>
         </is>
       </c>
-      <c r="B38" s="13" t="inlineStr"/>
-      <c r="C38" s="14" t="inlineStr">
+      <c r="B38" s="21" t="inlineStr"/>
+      <c r="C38" s="22" t="inlineStr">
         <is>
           <t>03/Jun/2025</t>
         </is>
       </c>
-      <c r="D38" s="12" t="inlineStr">
+      <c r="D38" s="20" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E38" s="15" t="inlineStr">
+      <c r="E38" s="23" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F38" s="12" t="inlineStr"/>
-      <c r="G38" s="12" t="inlineStr"/>
-      <c r="H38" s="16" t="inlineStr">
+      <c r="F38" s="20" t="inlineStr"/>
+      <c r="G38" s="20" t="inlineStr"/>
+      <c r="H38" s="24" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I38" s="12" t="inlineStr">
+      <c r="I38" s="20" t="inlineStr">
         <is>
           <t>70397</t>
         </is>
       </c>
-      <c r="J38" s="17" t="inlineStr">
+      <c r="J38" s="25" t="inlineStr">
         <is>
           <t>100000</t>
         </is>
       </c>
-      <c r="K38" s="12" t="inlineStr"/>
-      <c r="L38" s="12" t="inlineStr">
+      <c r="K38" s="20" t="inlineStr"/>
+      <c r="L38" s="20" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="12" t="inlineStr">
+      <c r="A39" s="20" t="inlineStr">
         <is>
           <t>M076</t>
         </is>
       </c>
-      <c r="B39" s="13" t="inlineStr">
+      <c r="B39" s="21" t="inlineStr">
         <is>
           <t>Interunit Loan Match: MDB#0331
 Lender Amount: 100000.00
 Borrower Amount: 100000.00</t>
         </is>
       </c>
-      <c r="C39" s="12" t="inlineStr"/>
-      <c r="D39" s="12" t="inlineStr"/>
-      <c r="E39" s="18" t="inlineStr">
+      <c r="C39" s="20" t="inlineStr"/>
+      <c r="D39" s="20" t="inlineStr"/>
+      <c r="E39" s="26" t="inlineStr">
         <is>
           <t>Being the amount paid to BSRM Wires Limited. Supply of , Invoice Number:  424001088, Challan Number: 3060537, Work Order Number: DES/PO/2024/11/30582, BA Team (A), Company Unit: Concrete Pole &amp; Pile, Project Name : DESCO SPC Pole (GD-4), Work Order date: 2024-11-27, Goods Received Date: 2024-12-03, Work Order Value: 204668.0, Total Bill Amount: 199329.0, TDS Deduction Amount: 0.0, VDS Deduction Amount: 0.0</t>
         </is>
       </c>
-      <c r="F39" s="12" t="inlineStr"/>
-      <c r="G39" s="12" t="inlineStr"/>
-      <c r="H39" s="12" t="inlineStr"/>
-      <c r="I39" s="12" t="inlineStr"/>
-      <c r="J39" s="12" t="inlineStr"/>
-      <c r="K39" s="12" t="inlineStr"/>
-      <c r="L39" s="12" t="inlineStr">
+      <c r="F39" s="20" t="inlineStr"/>
+      <c r="G39" s="20" t="inlineStr"/>
+      <c r="H39" s="20" t="inlineStr"/>
+      <c r="I39" s="20" t="inlineStr"/>
+      <c r="J39" s="20" t="inlineStr"/>
+      <c r="K39" s="20" t="inlineStr"/>
+      <c r="L39" s="20" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="12" t="inlineStr">
+      <c r="A40" s="20" t="inlineStr">
         <is>
           <t>M076</t>
         </is>
       </c>
-      <c r="B40" s="13" t="inlineStr"/>
-      <c r="C40" s="12" t="inlineStr"/>
-      <c r="D40" s="12" t="inlineStr">
+      <c r="B40" s="21" t="inlineStr"/>
+      <c r="C40" s="20" t="inlineStr"/>
+      <c r="D40" s="20" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E40" s="19" t="inlineStr">
+      <c r="E40" s="27" t="inlineStr">
         <is>
           <t>ziaul</t>
         </is>
       </c>
-      <c r="F40" s="12" t="inlineStr"/>
-      <c r="G40" s="12" t="inlineStr"/>
-      <c r="H40" s="12" t="inlineStr"/>
-      <c r="I40" s="12" t="inlineStr"/>
-      <c r="J40" s="12" t="inlineStr"/>
-      <c r="K40" s="12" t="inlineStr"/>
-      <c r="L40" s="12" t="inlineStr">
+      <c r="F40" s="20" t="inlineStr"/>
+      <c r="G40" s="20" t="inlineStr"/>
+      <c r="H40" s="20" t="inlineStr"/>
+      <c r="I40" s="20" t="inlineStr"/>
+      <c r="J40" s="20" t="inlineStr"/>
+      <c r="K40" s="20" t="inlineStr"/>
+      <c r="L40" s="20" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
@@ -2181,691 +2204,760 @@
       <c r="L48" s="1" t="inlineStr"/>
     </row>
     <row r="49">
-      <c r="A49" s="20" t="inlineStr">
+      <c r="A49" s="12" t="inlineStr">
         <is>
           <t>M078</t>
         </is>
       </c>
-      <c r="B49" s="21" t="inlineStr"/>
-      <c r="C49" s="22" t="inlineStr">
+      <c r="B49" s="13" t="inlineStr"/>
+      <c r="C49" s="14" t="inlineStr">
         <is>
           <t>04/Jun/2025</t>
         </is>
       </c>
-      <c r="D49" s="20" t="inlineStr">
+      <c r="D49" s="12" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E49" s="23" t="inlineStr">
+      <c r="E49" s="15" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F49" s="20" t="inlineStr"/>
-      <c r="G49" s="20" t="inlineStr"/>
-      <c r="H49" s="24" t="inlineStr">
+      <c r="F49" s="12" t="inlineStr"/>
+      <c r="G49" s="12" t="inlineStr"/>
+      <c r="H49" s="16" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I49" s="20" t="inlineStr">
+      <c r="I49" s="12" t="inlineStr">
         <is>
           <t>70400</t>
         </is>
       </c>
-      <c r="J49" s="25" t="inlineStr">
+      <c r="J49" s="17" t="inlineStr">
         <is>
           <t>200000</t>
         </is>
       </c>
-      <c r="K49" s="20" t="inlineStr"/>
-      <c r="L49" s="20" t="inlineStr">
+      <c r="K49" s="12" t="inlineStr"/>
+      <c r="L49" s="12" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="20" t="inlineStr">
+      <c r="A50" s="12" t="inlineStr">
         <is>
           <t>M078</t>
         </is>
       </c>
-      <c r="B50" s="21" t="inlineStr">
+      <c r="B50" s="13" t="inlineStr">
         <is>
           <t>Interunit Loan Match: MDB#0331
 Lender Amount: 200000.00
 Borrower Amount: 200000.00</t>
         </is>
       </c>
-      <c r="C50" s="20" t="inlineStr"/>
-      <c r="D50" s="20" t="inlineStr"/>
-      <c r="E50" s="26" t="inlineStr">
+      <c r="C50" s="12" t="inlineStr"/>
+      <c r="D50" s="12" t="inlineStr"/>
+      <c r="E50" s="18" t="inlineStr">
         <is>
           <t>Being the amount paid to M/S. Sweet Enterprise. Supply of , Invoice Number:  053, Challan Number: 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757,1741, Work Order Number: PBS/PO/2024/10/29823, BA Team (A), Company Unit: Concrete Pole &amp; Pile, Project Name : PBSF-G-260 (ID:949763), Work Order date: 2024-10-03, Goods Received Date: 2024-10-12, Work Order Value: 1800000.0, Total Bill Amount: 703890.0, TDS Deduction Amount: 0.0, VDS Deduction Amount: 0.0</t>
         </is>
       </c>
-      <c r="F50" s="20" t="inlineStr"/>
-      <c r="G50" s="20" t="inlineStr"/>
-      <c r="H50" s="20" t="inlineStr"/>
-      <c r="I50" s="20" t="inlineStr"/>
-      <c r="J50" s="20" t="inlineStr"/>
-      <c r="K50" s="20" t="inlineStr"/>
-      <c r="L50" s="20" t="inlineStr">
+      <c r="F50" s="12" t="inlineStr"/>
+      <c r="G50" s="12" t="inlineStr"/>
+      <c r="H50" s="12" t="inlineStr"/>
+      <c r="I50" s="12" t="inlineStr"/>
+      <c r="J50" s="12" t="inlineStr"/>
+      <c r="K50" s="12" t="inlineStr"/>
+      <c r="L50" s="12" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="20" t="inlineStr">
+      <c r="A51" s="12" t="inlineStr">
         <is>
           <t>M078</t>
         </is>
       </c>
-      <c r="B51" s="21" t="inlineStr"/>
-      <c r="C51" s="20" t="inlineStr"/>
-      <c r="D51" s="20" t="inlineStr">
+      <c r="B51" s="13" t="inlineStr"/>
+      <c r="C51" s="12" t="inlineStr"/>
+      <c r="D51" s="12" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E51" s="27" t="inlineStr">
+      <c r="E51" s="19" t="inlineStr">
         <is>
           <t>ziaul</t>
         </is>
       </c>
-      <c r="F51" s="20" t="inlineStr"/>
-      <c r="G51" s="20" t="inlineStr"/>
-      <c r="H51" s="20" t="inlineStr"/>
-      <c r="I51" s="20" t="inlineStr"/>
-      <c r="J51" s="20" t="inlineStr"/>
-      <c r="K51" s="20" t="inlineStr"/>
-      <c r="L51" s="20" t="inlineStr">
+      <c r="F51" s="12" t="inlineStr"/>
+      <c r="G51" s="12" t="inlineStr"/>
+      <c r="H51" s="12" t="inlineStr"/>
+      <c r="I51" s="12" t="inlineStr"/>
+      <c r="J51" s="12" t="inlineStr"/>
+      <c r="K51" s="12" t="inlineStr"/>
+      <c r="L51" s="12" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="12" t="inlineStr">
+      <c r="A52" s="20" t="inlineStr">
         <is>
           <t>M123</t>
         </is>
       </c>
-      <c r="B52" s="13" t="inlineStr"/>
-      <c r="C52" s="14" t="inlineStr">
+      <c r="B52" s="21" t="inlineStr"/>
+      <c r="C52" s="22" t="inlineStr">
         <is>
           <t>04/Jun/2025</t>
         </is>
       </c>
-      <c r="D52" s="12" t="inlineStr">
+      <c r="D52" s="20" t="inlineStr">
         <is>
           <t>Dr</t>
         </is>
       </c>
-      <c r="E52" s="15" t="inlineStr">
+      <c r="E52" s="23" t="inlineStr">
         <is>
           <t>Eastern Bank PLC-OD-A/C-1012040000125</t>
         </is>
       </c>
-      <c r="F52" s="12" t="inlineStr"/>
-      <c r="G52" s="12" t="inlineStr"/>
-      <c r="H52" s="16" t="inlineStr">
+      <c r="F52" s="20" t="inlineStr"/>
+      <c r="G52" s="20" t="inlineStr"/>
+      <c r="H52" s="24" t="inlineStr">
         <is>
           <t>Receipt</t>
         </is>
       </c>
-      <c r="I52" s="12" t="inlineStr">
+      <c r="I52" s="20" t="inlineStr">
         <is>
           <t>941</t>
         </is>
       </c>
-      <c r="J52" s="12" t="inlineStr"/>
-      <c r="K52" s="17" t="inlineStr">
+      <c r="J52" s="20" t="inlineStr"/>
+      <c r="K52" s="25" t="inlineStr">
         <is>
           <t>41625247.63</t>
         </is>
       </c>
-      <c r="L52" s="12" t="inlineStr">
+      <c r="L52" s="20" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="12" t="inlineStr">
+      <c r="A53" s="20" t="inlineStr">
         <is>
           <t>M123</t>
         </is>
       </c>
-      <c r="B53" s="13" t="inlineStr">
+      <c r="B53" s="21" t="inlineStr">
         <is>
           <t>USD Match: $.789,663.20
 Lender Amount: 41625247.63
 Borrower Amount: 41625247.63</t>
         </is>
       </c>
-      <c r="C53" s="12" t="inlineStr"/>
-      <c r="D53" s="12" t="inlineStr"/>
-      <c r="E53" s="18" t="inlineStr">
+      <c r="C53" s="20" t="inlineStr"/>
+      <c r="D53" s="20" t="inlineStr"/>
+      <c r="E53" s="26" t="inlineStr">
         <is>
           <t>Amount received agst Contract no.MCEP/BREB/DMD-SPC-G-24-Lot-1/2023-2024. Date.07.07.2024 This amount actually Pole Unit but deposit in Geo Textile Unit. Total bill amount $.789,663.20/- But ($.443,663.42+$6,400) Deposit in Geo Textile Unit. Remaining   $339520.78 Deposit in Steel Unit. Bank charge-$80. Rate.122.60</t>
         </is>
       </c>
-      <c r="F53" s="12" t="inlineStr"/>
-      <c r="G53" s="12" t="inlineStr"/>
-      <c r="H53" s="12" t="inlineStr"/>
-      <c r="I53" s="12" t="inlineStr"/>
-      <c r="J53" s="12" t="inlineStr"/>
-      <c r="K53" s="12" t="inlineStr"/>
-      <c r="L53" s="12" t="inlineStr">
+      <c r="F53" s="20" t="inlineStr"/>
+      <c r="G53" s="20" t="inlineStr"/>
+      <c r="H53" s="20" t="inlineStr"/>
+      <c r="I53" s="20" t="inlineStr"/>
+      <c r="J53" s="20" t="inlineStr"/>
+      <c r="K53" s="20" t="inlineStr"/>
+      <c r="L53" s="20" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="12" t="inlineStr">
+      <c r="A54" s="20" t="inlineStr">
         <is>
           <t>M123</t>
         </is>
       </c>
-      <c r="B54" s="13" t="inlineStr"/>
-      <c r="C54" s="12" t="inlineStr"/>
-      <c r="D54" s="12" t="inlineStr">
+      <c r="B54" s="21" t="inlineStr"/>
+      <c r="C54" s="20" t="inlineStr"/>
+      <c r="D54" s="20" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E54" s="19" t="inlineStr">
+      <c r="E54" s="27" t="inlineStr">
         <is>
           <t>sayeda</t>
         </is>
       </c>
-      <c r="F54" s="12" t="inlineStr"/>
-      <c r="G54" s="12" t="inlineStr"/>
-      <c r="H54" s="12" t="inlineStr"/>
-      <c r="I54" s="12" t="inlineStr"/>
-      <c r="J54" s="12" t="inlineStr"/>
-      <c r="K54" s="12" t="inlineStr"/>
-      <c r="L54" s="12" t="inlineStr">
+      <c r="F54" s="20" t="inlineStr"/>
+      <c r="G54" s="20" t="inlineStr"/>
+      <c r="H54" s="20" t="inlineStr"/>
+      <c r="I54" s="20" t="inlineStr"/>
+      <c r="J54" s="20" t="inlineStr"/>
+      <c r="K54" s="20" t="inlineStr"/>
+      <c r="L54" s="20" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="20" t="inlineStr">
+      <c r="A55" s="12" t="inlineStr">
         <is>
           <t>M002</t>
         </is>
       </c>
-      <c r="B55" s="21" t="inlineStr"/>
-      <c r="C55" s="22" t="inlineStr">
+      <c r="B55" s="13" t="inlineStr"/>
+      <c r="C55" s="14" t="inlineStr">
         <is>
           <t>04/Jun/2025</t>
         </is>
       </c>
-      <c r="D55" s="20" t="inlineStr">
+      <c r="D55" s="12" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E55" s="23" t="inlineStr">
+      <c r="E55" s="15" t="inlineStr">
         <is>
           <t>Mutual Trust Bank Ltd-SND-002-0320004355</t>
         </is>
       </c>
-      <c r="F55" s="20" t="inlineStr"/>
-      <c r="G55" s="20" t="inlineStr"/>
-      <c r="H55" s="24" t="inlineStr">
+      <c r="F55" s="12" t="inlineStr"/>
+      <c r="G55" s="12" t="inlineStr"/>
+      <c r="H55" s="16" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I55" s="20" t="inlineStr">
+      <c r="I55" s="12" t="inlineStr">
         <is>
           <t>70804</t>
         </is>
       </c>
-      <c r="J55" s="25" t="inlineStr">
+      <c r="J55" s="17" t="inlineStr">
         <is>
           <t>36600000</t>
         </is>
       </c>
-      <c r="K55" s="20" t="inlineStr"/>
-      <c r="L55" s="20" t="inlineStr">
+      <c r="K55" s="12" t="inlineStr"/>
+      <c r="L55" s="12" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="20" t="inlineStr">
+      <c r="A56" s="12" t="inlineStr">
         <is>
           <t>M002</t>
         </is>
       </c>
-      <c r="B56" s="21" t="inlineStr">
+      <c r="B56" s="13" t="inlineStr">
         <is>
           <t>USD Match: $300,000
 Lender Amount: 36600000.00
 Borrower Amount: 36600000.00</t>
         </is>
       </c>
-      <c r="C56" s="20" t="inlineStr"/>
-      <c r="D56" s="20" t="inlineStr"/>
-      <c r="E56" s="26" t="inlineStr">
+      <c r="C56" s="12" t="inlineStr"/>
+      <c r="D56" s="12" t="inlineStr"/>
+      <c r="E56" s="18" t="inlineStr">
         <is>
           <t>Amount pais to Sundry Party-Castle Construction Co.Ltd. $300,000 @ Tk.122/-</t>
         </is>
       </c>
-      <c r="F56" s="20" t="inlineStr"/>
-      <c r="G56" s="20" t="inlineStr"/>
-      <c r="H56" s="20" t="inlineStr"/>
-      <c r="I56" s="20" t="inlineStr"/>
-      <c r="J56" s="20" t="inlineStr"/>
-      <c r="K56" s="20" t="inlineStr"/>
-      <c r="L56" s="20" t="inlineStr">
+      <c r="F56" s="12" t="inlineStr"/>
+      <c r="G56" s="12" t="inlineStr"/>
+      <c r="H56" s="12" t="inlineStr"/>
+      <c r="I56" s="12" t="inlineStr"/>
+      <c r="J56" s="12" t="inlineStr"/>
+      <c r="K56" s="12" t="inlineStr"/>
+      <c r="L56" s="12" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="20" t="inlineStr">
+      <c r="A57" s="12" t="inlineStr">
         <is>
           <t>M002</t>
         </is>
       </c>
-      <c r="B57" s="21" t="inlineStr"/>
-      <c r="C57" s="20" t="inlineStr"/>
-      <c r="D57" s="20" t="inlineStr">
+      <c r="B57" s="13" t="inlineStr"/>
+      <c r="C57" s="12" t="inlineStr"/>
+      <c r="D57" s="12" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E57" s="27" t="inlineStr">
+      <c r="E57" s="19" t="inlineStr">
         <is>
           <t>ashiq</t>
         </is>
       </c>
-      <c r="F57" s="20" t="inlineStr"/>
-      <c r="G57" s="20" t="inlineStr"/>
-      <c r="H57" s="20" t="inlineStr"/>
-      <c r="I57" s="20" t="inlineStr"/>
-      <c r="J57" s="20" t="inlineStr"/>
-      <c r="K57" s="20" t="inlineStr"/>
-      <c r="L57" s="20" t="inlineStr">
+      <c r="F57" s="12" t="inlineStr"/>
+      <c r="G57" s="12" t="inlineStr"/>
+      <c r="H57" s="12" t="inlineStr"/>
+      <c r="I57" s="12" t="inlineStr"/>
+      <c r="J57" s="12" t="inlineStr"/>
+      <c r="K57" s="12" t="inlineStr"/>
+      <c r="L57" s="12" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="12" t="inlineStr">
+      <c r="A58" s="20" t="inlineStr">
         <is>
           <t>M004</t>
         </is>
       </c>
-      <c r="B58" s="13" t="inlineStr"/>
-      <c r="C58" s="14" t="inlineStr">
+      <c r="B58" s="21" t="inlineStr"/>
+      <c r="C58" s="22" t="inlineStr">
         <is>
           <t>05/Jun/2025</t>
         </is>
       </c>
-      <c r="D58" s="12" t="inlineStr">
+      <c r="D58" s="20" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E58" s="15" t="inlineStr">
+      <c r="E58" s="23" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F58" s="12" t="inlineStr"/>
-      <c r="G58" s="12" t="inlineStr"/>
-      <c r="H58" s="16" t="inlineStr">
+      <c r="F58" s="20" t="inlineStr"/>
+      <c r="G58" s="20" t="inlineStr"/>
+      <c r="H58" s="24" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I58" s="12" t="inlineStr">
+      <c r="I58" s="20" t="inlineStr">
         <is>
           <t>70845</t>
         </is>
       </c>
-      <c r="J58" s="17" t="inlineStr">
+      <c r="J58" s="25" t="inlineStr">
         <is>
           <t>62525</t>
         </is>
       </c>
-      <c r="K58" s="12" t="inlineStr"/>
-      <c r="L58" s="12" t="inlineStr">
+      <c r="K58" s="20" t="inlineStr"/>
+      <c r="L58" s="20" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="12" t="inlineStr">
+      <c r="A59" s="20" t="inlineStr">
         <is>
           <t>M004</t>
         </is>
       </c>
-      <c r="B59" s="13" t="inlineStr">
+      <c r="B59" s="21" t="inlineStr">
         <is>
           <t>Narration Match
 Lender Amount: 62525.00
 Borrower Amount: 62525.00</t>
         </is>
       </c>
-      <c r="C59" s="12" t="inlineStr"/>
-      <c r="D59" s="12" t="inlineStr"/>
-      <c r="E59" s="18" t="inlineStr">
+      <c r="C59" s="20" t="inlineStr"/>
+      <c r="D59" s="20" t="inlineStr"/>
+      <c r="E59" s="26" t="inlineStr">
         <is>
           <t>Being the amount paid to Lube Corner- Supply of consumble , Bill NO 1394:   Challan Number:   Manual PO [ CCEL Reno/PO/20245//8/87247(E)].  BA Team (A), Company Unit: Concrete Pole &amp; Pile, Project Name :  SPC Pole ( CCEL) Renovation. actual VN : 23011 in pole unit.</t>
         </is>
       </c>
-      <c r="F59" s="12" t="inlineStr"/>
-      <c r="G59" s="12" t="inlineStr"/>
-      <c r="H59" s="12" t="inlineStr"/>
-      <c r="I59" s="12" t="inlineStr"/>
-      <c r="J59" s="12" t="inlineStr"/>
-      <c r="K59" s="12" t="inlineStr"/>
-      <c r="L59" s="12" t="inlineStr">
+      <c r="F59" s="20" t="inlineStr"/>
+      <c r="G59" s="20" t="inlineStr"/>
+      <c r="H59" s="20" t="inlineStr"/>
+      <c r="I59" s="20" t="inlineStr"/>
+      <c r="J59" s="20" t="inlineStr"/>
+      <c r="K59" s="20" t="inlineStr"/>
+      <c r="L59" s="20" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="12" t="inlineStr">
+      <c r="A60" s="20" t="inlineStr">
         <is>
           <t>M004</t>
         </is>
       </c>
-      <c r="B60" s="13" t="inlineStr"/>
-      <c r="C60" s="12" t="inlineStr"/>
-      <c r="D60" s="12" t="inlineStr">
+      <c r="B60" s="21" t="inlineStr"/>
+      <c r="C60" s="20" t="inlineStr"/>
+      <c r="D60" s="20" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E60" s="19" t="inlineStr">
+      <c r="E60" s="27" t="inlineStr">
         <is>
           <t>nur.hossain</t>
         </is>
       </c>
-      <c r="F60" s="12" t="inlineStr"/>
-      <c r="G60" s="12" t="inlineStr"/>
-      <c r="H60" s="12" t="inlineStr"/>
-      <c r="I60" s="12" t="inlineStr"/>
-      <c r="J60" s="12" t="inlineStr"/>
-      <c r="K60" s="12" t="inlineStr"/>
-      <c r="L60" s="12" t="inlineStr">
+      <c r="F60" s="20" t="inlineStr"/>
+      <c r="G60" s="20" t="inlineStr"/>
+      <c r="H60" s="20" t="inlineStr"/>
+      <c r="I60" s="20" t="inlineStr"/>
+      <c r="J60" s="20" t="inlineStr"/>
+      <c r="K60" s="20" t="inlineStr"/>
+      <c r="L60" s="20" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="inlineStr"/>
-      <c r="B61" s="2" t="inlineStr"/>
-      <c r="C61" s="6" t="inlineStr">
+      <c r="A61" s="12" t="inlineStr">
+        <is>
+          <t>M127</t>
+        </is>
+      </c>
+      <c r="B61" s="13" t="inlineStr"/>
+      <c r="C61" s="14" t="inlineStr">
         <is>
           <t>05/Jun/2025</t>
         </is>
       </c>
-      <c r="D61" s="1" t="inlineStr">
+      <c r="D61" s="12" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E61" s="7" t="inlineStr">
+      <c r="E61" s="15" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F61" s="1" t="inlineStr"/>
-      <c r="G61" s="1" t="inlineStr"/>
-      <c r="H61" s="9" t="inlineStr">
+      <c r="F61" s="12" t="inlineStr"/>
+      <c r="G61" s="12" t="inlineStr"/>
+      <c r="H61" s="16" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I61" s="1" t="inlineStr">
+      <c r="I61" s="12" t="inlineStr">
         <is>
           <t>70846</t>
         </is>
       </c>
-      <c r="J61" s="8" t="inlineStr">
+      <c r="J61" s="17" t="inlineStr">
         <is>
           <t>20000</t>
         </is>
       </c>
-      <c r="K61" s="1" t="inlineStr"/>
-      <c r="L61" s="1" t="inlineStr"/>
+      <c r="K61" s="12" t="inlineStr"/>
+      <c r="L61" s="12" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="inlineStr"/>
-      <c r="B62" s="2" t="inlineStr">
-        <is>
-          <t>Unmatched Record
-Reasons:
-1. Amounts don't match: 20000 vs 10562.5
-2. Amounts don't match: 20000 vs 2700</t>
-        </is>
-      </c>
-      <c r="C62" s="1" t="inlineStr"/>
-      <c r="D62" s="1" t="inlineStr"/>
-      <c r="E62" s="10" t="inlineStr">
+      <c r="A62" s="12" t="inlineStr">
+        <is>
+          <t>M127</t>
+        </is>
+      </c>
+      <c r="B62" s="13" t="inlineStr">
+        <is>
+          <t>Manual Match
+Lender Amount: 20000.00
+Borrower Amount: 20000.00</t>
+        </is>
+      </c>
+      <c r="C62" s="12" t="inlineStr"/>
+      <c r="D62" s="12" t="inlineStr"/>
+      <c r="E62" s="18" t="inlineStr">
         <is>
           <t>Being the amount paid to-Chemitec -supply of consumble items , Bill NO 009:   Challan Number:   Manual PO [ CCEL Reno/PO/2024/8/87251)].  BA Team (A), Company Unit: Concrete Pole &amp; Pile, Project Name :  SPC Pole ( CCEL) Renovation. Actual VN:23018 in pole unite</t>
         </is>
       </c>
-      <c r="F62" s="1" t="inlineStr"/>
-      <c r="G62" s="1" t="inlineStr"/>
-      <c r="H62" s="1" t="inlineStr"/>
-      <c r="I62" s="1" t="inlineStr"/>
-      <c r="J62" s="1" t="inlineStr"/>
-      <c r="K62" s="1" t="inlineStr"/>
-      <c r="L62" s="1" t="inlineStr"/>
+      <c r="F62" s="12" t="inlineStr"/>
+      <c r="G62" s="12" t="inlineStr"/>
+      <c r="H62" s="12" t="inlineStr"/>
+      <c r="I62" s="12" t="inlineStr"/>
+      <c r="J62" s="12" t="inlineStr"/>
+      <c r="K62" s="12" t="inlineStr"/>
+      <c r="L62" s="12" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="inlineStr"/>
-      <c r="B63" s="2" t="inlineStr"/>
-      <c r="C63" s="1" t="inlineStr"/>
-      <c r="D63" s="1" t="inlineStr">
+      <c r="A63" s="12" t="inlineStr">
+        <is>
+          <t>M127</t>
+        </is>
+      </c>
+      <c r="B63" s="13" t="inlineStr"/>
+      <c r="C63" s="12" t="inlineStr"/>
+      <c r="D63" s="12" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E63" s="11" t="inlineStr">
+      <c r="E63" s="19" t="inlineStr">
         <is>
           <t>nur.hossain</t>
         </is>
       </c>
-      <c r="F63" s="1" t="inlineStr"/>
-      <c r="G63" s="1" t="inlineStr"/>
-      <c r="H63" s="1" t="inlineStr"/>
-      <c r="I63" s="1" t="inlineStr"/>
-      <c r="J63" s="1" t="inlineStr"/>
-      <c r="K63" s="1" t="inlineStr"/>
-      <c r="L63" s="1" t="inlineStr"/>
+      <c r="F63" s="12" t="inlineStr"/>
+      <c r="G63" s="12" t="inlineStr"/>
+      <c r="H63" s="12" t="inlineStr"/>
+      <c r="I63" s="12" t="inlineStr"/>
+      <c r="J63" s="12" t="inlineStr"/>
+      <c r="K63" s="12" t="inlineStr"/>
+      <c r="L63" s="12" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="inlineStr"/>
-      <c r="B64" s="2" t="inlineStr"/>
-      <c r="C64" s="6" t="inlineStr">
+      <c r="A64" s="20" t="inlineStr">
+        <is>
+          <t>M128</t>
+        </is>
+      </c>
+      <c r="B64" s="21" t="inlineStr"/>
+      <c r="C64" s="22" t="inlineStr">
         <is>
           <t>05/Jun/2025</t>
         </is>
       </c>
-      <c r="D64" s="1" t="inlineStr">
+      <c r="D64" s="20" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E64" s="7" t="inlineStr">
+      <c r="E64" s="23" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F64" s="1" t="inlineStr"/>
-      <c r="G64" s="1" t="inlineStr"/>
-      <c r="H64" s="9" t="inlineStr">
+      <c r="F64" s="20" t="inlineStr"/>
+      <c r="G64" s="20" t="inlineStr"/>
+      <c r="H64" s="24" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I64" s="1" t="inlineStr">
+      <c r="I64" s="20" t="inlineStr">
         <is>
           <t>70847</t>
         </is>
       </c>
-      <c r="J64" s="8" t="inlineStr">
+      <c r="J64" s="25" t="inlineStr">
         <is>
           <t>17500</t>
         </is>
       </c>
-      <c r="K64" s="1" t="inlineStr"/>
-      <c r="L64" s="1" t="inlineStr"/>
+      <c r="K64" s="20" t="inlineStr"/>
+      <c r="L64" s="20" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="inlineStr"/>
-      <c r="B65" s="2" t="inlineStr">
-        <is>
-          <t>Unmatched Record
-Reasons:
-1. Amounts don't match: 17500 vs 10562.5
-2. Amounts don't match: 17500 vs 2700</t>
-        </is>
-      </c>
-      <c r="C65" s="1" t="inlineStr"/>
-      <c r="D65" s="1" t="inlineStr"/>
-      <c r="E65" s="10" t="inlineStr">
+      <c r="A65" s="20" t="inlineStr">
+        <is>
+          <t>M128</t>
+        </is>
+      </c>
+      <c r="B65" s="21" t="inlineStr">
+        <is>
+          <t>Manual Match
+Lender Amount: 17500.00
+Borrower Amount: 17500.00</t>
+        </is>
+      </c>
+      <c r="C65" s="20" t="inlineStr"/>
+      <c r="D65" s="20" t="inlineStr"/>
+      <c r="E65" s="26" t="inlineStr">
         <is>
           <t>Being the amount -Safe Construction Solutions  to . against purchase CONSUMBLE ITEMS,    Challan Number:   Manual PO [ CCEL/Reno//PO///2024/9/21824-C] .bill no: 7951.  BA Team -Civil PEB unit. Company Unit: Concrete Pole &amp; Pile, Project Name :  SPC Pole ( CCEL) Renovation Actual VN: 23042 in pole unit</t>
         </is>
       </c>
-      <c r="F65" s="1" t="inlineStr"/>
-      <c r="G65" s="1" t="inlineStr"/>
-      <c r="H65" s="1" t="inlineStr"/>
-      <c r="I65" s="1" t="inlineStr"/>
-      <c r="J65" s="1" t="inlineStr"/>
-      <c r="K65" s="1" t="inlineStr"/>
-      <c r="L65" s="1" t="inlineStr"/>
+      <c r="F65" s="20" t="inlineStr"/>
+      <c r="G65" s="20" t="inlineStr"/>
+      <c r="H65" s="20" t="inlineStr"/>
+      <c r="I65" s="20" t="inlineStr"/>
+      <c r="J65" s="20" t="inlineStr"/>
+      <c r="K65" s="20" t="inlineStr"/>
+      <c r="L65" s="20" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="inlineStr"/>
-      <c r="B66" s="2" t="inlineStr"/>
-      <c r="C66" s="1" t="inlineStr"/>
-      <c r="D66" s="1" t="inlineStr">
+      <c r="A66" s="20" t="inlineStr">
+        <is>
+          <t>M128</t>
+        </is>
+      </c>
+      <c r="B66" s="21" t="inlineStr"/>
+      <c r="C66" s="20" t="inlineStr"/>
+      <c r="D66" s="20" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E66" s="11" t="inlineStr">
+      <c r="E66" s="27" t="inlineStr">
         <is>
           <t>nur.hossain</t>
         </is>
       </c>
-      <c r="F66" s="1" t="inlineStr"/>
-      <c r="G66" s="1" t="inlineStr"/>
-      <c r="H66" s="1" t="inlineStr"/>
-      <c r="I66" s="1" t="inlineStr"/>
-      <c r="J66" s="1" t="inlineStr"/>
-      <c r="K66" s="1" t="inlineStr"/>
-      <c r="L66" s="1" t="inlineStr"/>
+      <c r="F66" s="20" t="inlineStr"/>
+      <c r="G66" s="20" t="inlineStr"/>
+      <c r="H66" s="20" t="inlineStr"/>
+      <c r="I66" s="20" t="inlineStr"/>
+      <c r="J66" s="20" t="inlineStr"/>
+      <c r="K66" s="20" t="inlineStr"/>
+      <c r="L66" s="20" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="inlineStr"/>
-      <c r="B67" s="2" t="inlineStr"/>
-      <c r="C67" s="6" t="inlineStr">
+      <c r="A67" s="12" t="inlineStr">
+        <is>
+          <t>M129</t>
+        </is>
+      </c>
+      <c r="B67" s="13" t="inlineStr"/>
+      <c r="C67" s="14" t="inlineStr">
         <is>
           <t>05/Jun/2025</t>
         </is>
       </c>
-      <c r="D67" s="1" t="inlineStr">
+      <c r="D67" s="12" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E67" s="7" t="inlineStr">
+      <c r="E67" s="15" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F67" s="1" t="inlineStr"/>
-      <c r="G67" s="1" t="inlineStr"/>
-      <c r="H67" s="9" t="inlineStr">
+      <c r="F67" s="12" t="inlineStr"/>
+      <c r="G67" s="12" t="inlineStr"/>
+      <c r="H67" s="16" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I67" s="1" t="inlineStr">
+      <c r="I67" s="12" t="inlineStr">
         <is>
           <t>70848</t>
         </is>
       </c>
-      <c r="J67" s="8" t="inlineStr">
+      <c r="J67" s="17" t="inlineStr">
         <is>
           <t>110839</t>
         </is>
       </c>
-      <c r="K67" s="1" t="inlineStr"/>
-      <c r="L67" s="1" t="inlineStr"/>
+      <c r="K67" s="12" t="inlineStr"/>
+      <c r="L67" s="12" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="inlineStr"/>
-      <c r="B68" s="2" t="inlineStr">
-        <is>
-          <t>Unmatched Record
-Reasons:
-1. Amounts don't match: 110839 vs 10562.5
-2. Amounts don't match: 110839 vs 2700</t>
-        </is>
-      </c>
-      <c r="C68" s="1" t="inlineStr"/>
-      <c r="D68" s="1" t="inlineStr"/>
-      <c r="E68" s="10" t="inlineStr">
+      <c r="A68" s="12" t="inlineStr">
+        <is>
+          <t>M129</t>
+        </is>
+      </c>
+      <c r="B68" s="13" t="inlineStr">
+        <is>
+          <t>Manual Match
+Lender Amount: 110839.00
+Borrower Amount: 110839.00</t>
+        </is>
+      </c>
+      <c r="C68" s="12" t="inlineStr"/>
+      <c r="D68" s="12" t="inlineStr"/>
+      <c r="E68" s="18" t="inlineStr">
         <is>
           <t>Being the amount paid to Pragati Life Insurance Limited agt. Group Insurance Renewal Bill. Bill No.: 00633 &amp; 00633-C. Bill period: 1 march -2025 to 28 feb -2026</t>
         </is>
       </c>
-      <c r="F68" s="1" t="inlineStr"/>
-      <c r="G68" s="1" t="inlineStr"/>
-      <c r="H68" s="1" t="inlineStr"/>
-      <c r="I68" s="1" t="inlineStr"/>
-      <c r="J68" s="1" t="inlineStr"/>
-      <c r="K68" s="1" t="inlineStr"/>
-      <c r="L68" s="1" t="inlineStr"/>
+      <c r="F68" s="12" t="inlineStr"/>
+      <c r="G68" s="12" t="inlineStr"/>
+      <c r="H68" s="12" t="inlineStr"/>
+      <c r="I68" s="12" t="inlineStr"/>
+      <c r="J68" s="12" t="inlineStr"/>
+      <c r="K68" s="12" t="inlineStr"/>
+      <c r="L68" s="12" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="inlineStr"/>
-      <c r="B69" s="2" t="inlineStr"/>
-      <c r="C69" s="1" t="inlineStr"/>
-      <c r="D69" s="1" t="inlineStr">
+      <c r="A69" s="12" t="inlineStr">
+        <is>
+          <t>M129</t>
+        </is>
+      </c>
+      <c r="B69" s="13" t="inlineStr"/>
+      <c r="C69" s="12" t="inlineStr"/>
+      <c r="D69" s="12" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E69" s="11" t="inlineStr">
+      <c r="E69" s="19" t="inlineStr">
         <is>
           <t>nur.hossain</t>
         </is>
       </c>
-      <c r="F69" s="1" t="inlineStr"/>
-      <c r="G69" s="1" t="inlineStr"/>
-      <c r="H69" s="1" t="inlineStr"/>
-      <c r="I69" s="1" t="inlineStr"/>
-      <c r="J69" s="1" t="inlineStr"/>
-      <c r="K69" s="1" t="inlineStr"/>
-      <c r="L69" s="1" t="inlineStr"/>
+      <c r="F69" s="12" t="inlineStr"/>
+      <c r="G69" s="12" t="inlineStr"/>
+      <c r="H69" s="12" t="inlineStr"/>
+      <c r="I69" s="12" t="inlineStr"/>
+      <c r="J69" s="12" t="inlineStr"/>
+      <c r="K69" s="12" t="inlineStr"/>
+      <c r="L69" s="12" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="20" t="inlineStr">
@@ -8242,516 +8334,540 @@
       </c>
     </row>
     <row r="221">
-      <c r="A221" s="1" t="inlineStr"/>
-      <c r="B221" s="2" t="inlineStr"/>
-      <c r="C221" s="6" t="inlineStr">
+      <c r="A221" s="20" t="inlineStr">
+        <is>
+          <t>M130</t>
+        </is>
+      </c>
+      <c r="B221" s="21" t="inlineStr"/>
+      <c r="C221" s="22" t="inlineStr">
         <is>
           <t>23/Jun/2025</t>
         </is>
       </c>
-      <c r="D221" s="1" t="inlineStr">
+      <c r="D221" s="20" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E221" s="7" t="inlineStr">
+      <c r="E221" s="23" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F221" s="1" t="inlineStr"/>
-      <c r="G221" s="1" t="inlineStr"/>
-      <c r="H221" s="9" t="inlineStr">
+      <c r="F221" s="20" t="inlineStr"/>
+      <c r="G221" s="20" t="inlineStr"/>
+      <c r="H221" s="24" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I221" s="1" t="inlineStr">
+      <c r="I221" s="20" t="inlineStr">
         <is>
           <t>70568</t>
         </is>
       </c>
-      <c r="J221" s="8" t="inlineStr">
+      <c r="J221" s="25" t="inlineStr">
         <is>
           <t>24000000</t>
         </is>
       </c>
-      <c r="K221" s="1" t="inlineStr"/>
-      <c r="L221" s="1" t="inlineStr"/>
+      <c r="K221" s="20" t="inlineStr"/>
+      <c r="L221" s="20" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="222">
-      <c r="A222" s="1" t="inlineStr"/>
-      <c r="B222" s="2" t="inlineStr">
-        <is>
-          <t>Unmatched Record
-Reasons:
-1. Borrower's narration does not contain lender's short code</t>
-        </is>
-      </c>
-      <c r="C222" s="1" t="inlineStr"/>
-      <c r="D222" s="1" t="inlineStr"/>
-      <c r="E222" s="10" t="inlineStr">
+      <c r="A222" s="20" t="inlineStr">
+        <is>
+          <t>M130</t>
+        </is>
+      </c>
+      <c r="B222" s="21" t="inlineStr">
+        <is>
+          <t>Manual Match
+Lender Amount: 24000000.00
+Borrower Amount: 24000000.00</t>
+        </is>
+      </c>
+      <c r="C222" s="20" t="inlineStr"/>
+      <c r="D222" s="20" t="inlineStr"/>
+      <c r="E222" s="26" t="inlineStr">
         <is>
           <t>Interunit fund Transfer as Inter Unit Loan A/C-Pole Unit, MDBL#00304</t>
         </is>
       </c>
-      <c r="F222" s="1" t="inlineStr"/>
-      <c r="G222" s="1" t="inlineStr"/>
-      <c r="H222" s="1" t="inlineStr"/>
-      <c r="I222" s="1" t="inlineStr"/>
-      <c r="J222" s="1" t="inlineStr"/>
-      <c r="K222" s="1" t="inlineStr"/>
-      <c r="L222" s="1" t="inlineStr"/>
+      <c r="F222" s="20" t="inlineStr"/>
+      <c r="G222" s="20" t="inlineStr"/>
+      <c r="H222" s="20" t="inlineStr"/>
+      <c r="I222" s="20" t="inlineStr"/>
+      <c r="J222" s="20" t="inlineStr"/>
+      <c r="K222" s="20" t="inlineStr"/>
+      <c r="L222" s="20" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="223">
-      <c r="A223" s="1" t="inlineStr"/>
-      <c r="B223" s="2" t="inlineStr"/>
-      <c r="C223" s="1" t="inlineStr"/>
-      <c r="D223" s="1" t="inlineStr">
+      <c r="A223" s="20" t="inlineStr">
+        <is>
+          <t>M130</t>
+        </is>
+      </c>
+      <c r="B223" s="21" t="inlineStr"/>
+      <c r="C223" s="20" t="inlineStr"/>
+      <c r="D223" s="20" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E223" s="11" t="inlineStr">
+      <c r="E223" s="27" t="inlineStr">
         <is>
           <t>ashiq</t>
         </is>
       </c>
-      <c r="F223" s="1" t="inlineStr"/>
-      <c r="G223" s="1" t="inlineStr"/>
-      <c r="H223" s="1" t="inlineStr"/>
-      <c r="I223" s="1" t="inlineStr"/>
-      <c r="J223" s="1" t="inlineStr"/>
-      <c r="K223" s="1" t="inlineStr"/>
-      <c r="L223" s="1" t="inlineStr"/>
+      <c r="F223" s="20" t="inlineStr"/>
+      <c r="G223" s="20" t="inlineStr"/>
+      <c r="H223" s="20" t="inlineStr"/>
+      <c r="I223" s="20" t="inlineStr"/>
+      <c r="J223" s="20" t="inlineStr"/>
+      <c r="K223" s="20" t="inlineStr"/>
+      <c r="L223" s="20" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="224">
-      <c r="A224" s="20" t="inlineStr">
+      <c r="A224" s="12" t="inlineStr">
         <is>
           <t>M061</t>
         </is>
       </c>
-      <c r="B224" s="21" t="inlineStr"/>
-      <c r="C224" s="22" t="inlineStr">
+      <c r="B224" s="13" t="inlineStr"/>
+      <c r="C224" s="14" t="inlineStr">
         <is>
           <t>24/Jun/2025</t>
         </is>
       </c>
-      <c r="D224" s="20" t="inlineStr">
+      <c r="D224" s="12" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E224" s="23" t="inlineStr">
+      <c r="E224" s="15" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F224" s="20" t="inlineStr"/>
-      <c r="G224" s="20" t="inlineStr"/>
-      <c r="H224" s="24" t="inlineStr">
+      <c r="F224" s="12" t="inlineStr"/>
+      <c r="G224" s="12" t="inlineStr"/>
+      <c r="H224" s="16" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I224" s="20" t="inlineStr">
+      <c r="I224" s="12" t="inlineStr">
         <is>
           <t>70572</t>
         </is>
       </c>
-      <c r="J224" s="25" t="inlineStr">
+      <c r="J224" s="17" t="inlineStr">
         <is>
           <t>1235000</t>
         </is>
       </c>
-      <c r="K224" s="20" t="inlineStr"/>
-      <c r="L224" s="20" t="inlineStr">
+      <c r="K224" s="12" t="inlineStr"/>
+      <c r="L224" s="12" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="225">
-      <c r="A225" s="20" t="inlineStr">
+      <c r="A225" s="12" t="inlineStr">
         <is>
           <t>M061</t>
         </is>
       </c>
-      <c r="B225" s="21" t="inlineStr">
+      <c r="B225" s="13" t="inlineStr">
         <is>
           <t>LC Match: LC-187724010094/24
 Lender Amount: 1235000.00
 Borrower Amount: 1235000.00</t>
         </is>
       </c>
-      <c r="C225" s="20" t="inlineStr"/>
-      <c r="D225" s="20" t="inlineStr"/>
-      <c r="E225" s="26" t="inlineStr">
+      <c r="C225" s="12" t="inlineStr"/>
+      <c r="D225" s="12" t="inlineStr"/>
+      <c r="E225" s="18" t="inlineStr">
         <is>
           <t>Amount being paid as Port,Shipping &amp; Carrying charges agt LC-187724010094/24[Item-11,000 MT Crushed Stone-Project-G-24-Lot-1-Team-A]</t>
         </is>
       </c>
-      <c r="F225" s="20" t="inlineStr"/>
-      <c r="G225" s="20" t="inlineStr"/>
-      <c r="H225" s="20" t="inlineStr"/>
-      <c r="I225" s="20" t="inlineStr"/>
-      <c r="J225" s="20" t="inlineStr"/>
-      <c r="K225" s="20" t="inlineStr"/>
-      <c r="L225" s="20" t="inlineStr">
+      <c r="F225" s="12" t="inlineStr"/>
+      <c r="G225" s="12" t="inlineStr"/>
+      <c r="H225" s="12" t="inlineStr"/>
+      <c r="I225" s="12" t="inlineStr"/>
+      <c r="J225" s="12" t="inlineStr"/>
+      <c r="K225" s="12" t="inlineStr"/>
+      <c r="L225" s="12" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="226">
-      <c r="A226" s="20" t="inlineStr">
+      <c r="A226" s="12" t="inlineStr">
         <is>
           <t>M061</t>
         </is>
       </c>
-      <c r="B226" s="21" t="inlineStr"/>
-      <c r="C226" s="20" t="inlineStr"/>
-      <c r="D226" s="20" t="inlineStr">
+      <c r="B226" s="13" t="inlineStr"/>
+      <c r="C226" s="12" t="inlineStr"/>
+      <c r="D226" s="12" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E226" s="27" t="inlineStr">
+      <c r="E226" s="19" t="inlineStr">
         <is>
           <t>shabbirul</t>
         </is>
       </c>
-      <c r="F226" s="20" t="inlineStr"/>
-      <c r="G226" s="20" t="inlineStr"/>
-      <c r="H226" s="20" t="inlineStr"/>
-      <c r="I226" s="20" t="inlineStr"/>
-      <c r="J226" s="20" t="inlineStr"/>
-      <c r="K226" s="20" t="inlineStr"/>
-      <c r="L226" s="20" t="inlineStr">
+      <c r="F226" s="12" t="inlineStr"/>
+      <c r="G226" s="12" t="inlineStr"/>
+      <c r="H226" s="12" t="inlineStr"/>
+      <c r="I226" s="12" t="inlineStr"/>
+      <c r="J226" s="12" t="inlineStr"/>
+      <c r="K226" s="12" t="inlineStr"/>
+      <c r="L226" s="12" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="227">
-      <c r="A227" s="12" t="inlineStr">
+      <c r="A227" s="20" t="inlineStr">
         <is>
           <t>M121</t>
         </is>
       </c>
-      <c r="B227" s="13" t="inlineStr"/>
-      <c r="C227" s="14" t="inlineStr">
+      <c r="B227" s="21" t="inlineStr"/>
+      <c r="C227" s="22" t="inlineStr">
         <is>
           <t>25/Jun/2025</t>
         </is>
       </c>
-      <c r="D227" s="12" t="inlineStr">
+      <c r="D227" s="20" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E227" s="15" t="inlineStr">
+      <c r="E227" s="23" t="inlineStr">
         <is>
           <t>Eastern Bank,STD-1011220144056</t>
         </is>
       </c>
-      <c r="F227" s="12" t="inlineStr"/>
-      <c r="G227" s="12" t="inlineStr"/>
-      <c r="H227" s="16" t="inlineStr">
+      <c r="F227" s="20" t="inlineStr"/>
+      <c r="G227" s="20" t="inlineStr"/>
+      <c r="H227" s="24" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I227" s="12" t="inlineStr">
+      <c r="I227" s="20" t="inlineStr">
         <is>
           <t>70556</t>
         </is>
       </c>
-      <c r="J227" s="17" t="inlineStr">
+      <c r="J227" s="25" t="inlineStr">
         <is>
           <t>1300000</t>
         </is>
       </c>
-      <c r="K227" s="12" t="inlineStr"/>
-      <c r="L227" s="12" t="inlineStr">
+      <c r="K227" s="20" t="inlineStr"/>
+      <c r="L227" s="20" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="228">
-      <c r="A228" s="12" t="inlineStr">
+      <c r="A228" s="20" t="inlineStr">
         <is>
           <t>M121</t>
         </is>
       </c>
-      <c r="B228" s="13" t="inlineStr">
+      <c r="B228" s="21" t="inlineStr">
         <is>
           <t>Interunit Loan Match: EBL#4056
 Lender Amount: 1300000.00
 Borrower Amount: 1300000.00</t>
         </is>
       </c>
-      <c r="C228" s="12" t="inlineStr"/>
-      <c r="D228" s="12" t="inlineStr"/>
-      <c r="E228" s="18" t="inlineStr">
+      <c r="C228" s="20" t="inlineStr"/>
+      <c r="D228" s="20" t="inlineStr"/>
+      <c r="E228" s="26" t="inlineStr">
         <is>
           <t>Interunit fund transfer as Inter Unit Loan A/C-Pole Unit,EBL#44056</t>
         </is>
       </c>
-      <c r="F228" s="12" t="inlineStr"/>
-      <c r="G228" s="12" t="inlineStr"/>
-      <c r="H228" s="12" t="inlineStr"/>
-      <c r="I228" s="12" t="inlineStr"/>
-      <c r="J228" s="12" t="inlineStr"/>
-      <c r="K228" s="12" t="inlineStr"/>
-      <c r="L228" s="12" t="inlineStr">
+      <c r="F228" s="20" t="inlineStr"/>
+      <c r="G228" s="20" t="inlineStr"/>
+      <c r="H228" s="20" t="inlineStr"/>
+      <c r="I228" s="20" t="inlineStr"/>
+      <c r="J228" s="20" t="inlineStr"/>
+      <c r="K228" s="20" t="inlineStr"/>
+      <c r="L228" s="20" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="229">
-      <c r="A229" s="12" t="inlineStr">
+      <c r="A229" s="20" t="inlineStr">
         <is>
           <t>M121</t>
         </is>
       </c>
-      <c r="B229" s="13" t="inlineStr"/>
-      <c r="C229" s="12" t="inlineStr"/>
-      <c r="D229" s="12" t="inlineStr">
+      <c r="B229" s="21" t="inlineStr"/>
+      <c r="C229" s="20" t="inlineStr"/>
+      <c r="D229" s="20" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E229" s="19" t="inlineStr">
+      <c r="E229" s="27" t="inlineStr">
         <is>
           <t>ashiq</t>
         </is>
       </c>
-      <c r="F229" s="12" t="inlineStr"/>
-      <c r="G229" s="12" t="inlineStr"/>
-      <c r="H229" s="12" t="inlineStr"/>
-      <c r="I229" s="12" t="inlineStr"/>
-      <c r="J229" s="12" t="inlineStr"/>
-      <c r="K229" s="12" t="inlineStr"/>
-      <c r="L229" s="12" t="inlineStr">
+      <c r="F229" s="20" t="inlineStr"/>
+      <c r="G229" s="20" t="inlineStr"/>
+      <c r="H229" s="20" t="inlineStr"/>
+      <c r="I229" s="20" t="inlineStr"/>
+      <c r="J229" s="20" t="inlineStr"/>
+      <c r="K229" s="20" t="inlineStr"/>
+      <c r="L229" s="20" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="230">
-      <c r="A230" s="20" t="inlineStr">
+      <c r="A230" s="12" t="inlineStr">
         <is>
           <t>M063</t>
         </is>
       </c>
-      <c r="B230" s="21" t="inlineStr"/>
-      <c r="C230" s="22" t="inlineStr">
+      <c r="B230" s="13" t="inlineStr"/>
+      <c r="C230" s="14" t="inlineStr">
         <is>
           <t>26/Jun/2025</t>
         </is>
       </c>
-      <c r="D230" s="20" t="inlineStr">
+      <c r="D230" s="12" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E230" s="23" t="inlineStr">
+      <c r="E230" s="15" t="inlineStr">
         <is>
           <t>Prime Bank-CD-2126117010855</t>
         </is>
       </c>
-      <c r="F230" s="20" t="inlineStr"/>
-      <c r="G230" s="20" t="inlineStr"/>
-      <c r="H230" s="24" t="inlineStr">
+      <c r="F230" s="12" t="inlineStr"/>
+      <c r="G230" s="12" t="inlineStr"/>
+      <c r="H230" s="16" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I230" s="20" t="inlineStr">
+      <c r="I230" s="12" t="inlineStr">
         <is>
           <t>3188</t>
         </is>
       </c>
-      <c r="J230" s="25" t="inlineStr">
+      <c r="J230" s="17" t="inlineStr">
         <is>
           <t>43496089</t>
         </is>
       </c>
-      <c r="K230" s="20" t="inlineStr"/>
-      <c r="L230" s="20" t="inlineStr">
+      <c r="K230" s="12" t="inlineStr"/>
+      <c r="L230" s="12" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="231">
-      <c r="A231" s="20" t="inlineStr">
+      <c r="A231" s="12" t="inlineStr">
         <is>
           <t>M063</t>
         </is>
       </c>
-      <c r="B231" s="21" t="inlineStr">
+      <c r="B231" s="13" t="inlineStr">
         <is>
           <t>USD Match: $.789,663.20
 Lender Amount: 43496089.00
 Borrower Amount: 43496089.00</t>
         </is>
       </c>
-      <c r="C231" s="20" t="inlineStr"/>
-      <c r="D231" s="20" t="inlineStr"/>
-      <c r="E231" s="26" t="inlineStr">
+      <c r="C231" s="12" t="inlineStr"/>
+      <c r="D231" s="12" t="inlineStr"/>
+      <c r="E231" s="18" t="inlineStr">
         <is>
           <t>Amount paid agst Contract no.MCEP/BREB/DMD-SPC-G-24-Lot-1/2023-2024. Date.07.07.2024 This amount actually Pole Unit but deposit in Geo Textile Unit. Total bill amount $.789,663.20/- But ($.443,663.42+$6,400) Deposit in Geo Textile Unit. Remaining   $339520.78 Deposit in Steel Unit. Bank charge-$80. Rate.122.60, Total Received amount $.789583.20, Deposit amount JV partner Vicar Concrete Products $363,103.21 Remaing amount deposit in CIL.</t>
         </is>
       </c>
-      <c r="F231" s="20" t="inlineStr"/>
-      <c r="G231" s="20" t="inlineStr"/>
-      <c r="H231" s="20" t="inlineStr"/>
-      <c r="I231" s="20" t="inlineStr"/>
-      <c r="J231" s="20" t="inlineStr"/>
-      <c r="K231" s="20" t="inlineStr"/>
-      <c r="L231" s="20" t="inlineStr">
+      <c r="F231" s="12" t="inlineStr"/>
+      <c r="G231" s="12" t="inlineStr"/>
+      <c r="H231" s="12" t="inlineStr"/>
+      <c r="I231" s="12" t="inlineStr"/>
+      <c r="J231" s="12" t="inlineStr"/>
+      <c r="K231" s="12" t="inlineStr"/>
+      <c r="L231" s="12" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="232">
-      <c r="A232" s="20" t="inlineStr">
+      <c r="A232" s="12" t="inlineStr">
         <is>
           <t>M063</t>
         </is>
       </c>
-      <c r="B232" s="21" t="inlineStr"/>
-      <c r="C232" s="20" t="inlineStr"/>
-      <c r="D232" s="20" t="inlineStr">
+      <c r="B232" s="13" t="inlineStr"/>
+      <c r="C232" s="12" t="inlineStr"/>
+      <c r="D232" s="12" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E232" s="27" t="inlineStr">
+      <c r="E232" s="19" t="inlineStr">
         <is>
           <t>ashiq</t>
         </is>
       </c>
-      <c r="F232" s="20" t="inlineStr"/>
-      <c r="G232" s="20" t="inlineStr"/>
-      <c r="H232" s="20" t="inlineStr"/>
-      <c r="I232" s="20" t="inlineStr"/>
-      <c r="J232" s="20" t="inlineStr"/>
-      <c r="K232" s="20" t="inlineStr"/>
-      <c r="L232" s="20" t="inlineStr">
+      <c r="F232" s="12" t="inlineStr"/>
+      <c r="G232" s="12" t="inlineStr"/>
+      <c r="H232" s="12" t="inlineStr"/>
+      <c r="I232" s="12" t="inlineStr"/>
+      <c r="J232" s="12" t="inlineStr"/>
+      <c r="K232" s="12" t="inlineStr"/>
+      <c r="L232" s="12" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="233">
-      <c r="A233" s="12" t="inlineStr">
+      <c r="A233" s="20" t="inlineStr">
         <is>
           <t>M065</t>
         </is>
       </c>
-      <c r="B233" s="13" t="inlineStr"/>
-      <c r="C233" s="14" t="inlineStr">
+      <c r="B233" s="21" t="inlineStr"/>
+      <c r="C233" s="22" t="inlineStr">
         <is>
           <t>30/Jun/2025</t>
         </is>
       </c>
-      <c r="D233" s="12" t="inlineStr">
+      <c r="D233" s="20" t="inlineStr">
         <is>
           <t>Dr</t>
         </is>
       </c>
-      <c r="E233" s="15" t="inlineStr">
+      <c r="E233" s="23" t="inlineStr">
         <is>
           <t>Salary &amp; Allowance Payable</t>
         </is>
       </c>
-      <c r="F233" s="12" t="inlineStr"/>
-      <c r="G233" s="12" t="inlineStr"/>
-      <c r="H233" s="16" t="inlineStr">
+      <c r="F233" s="20" t="inlineStr"/>
+      <c r="G233" s="20" t="inlineStr"/>
+      <c r="H233" s="24" t="inlineStr">
         <is>
           <t>Journal</t>
         </is>
       </c>
-      <c r="I233" s="12" t="inlineStr">
+      <c r="I233" s="20" t="inlineStr">
         <is>
           <t>3855</t>
         </is>
       </c>
-      <c r="J233" s="12" t="inlineStr"/>
-      <c r="K233" s="17" t="inlineStr">
+      <c r="J233" s="20" t="inlineStr"/>
+      <c r="K233" s="25" t="inlineStr">
         <is>
           <t>20733</t>
         </is>
       </c>
-      <c r="L233" s="12" t="inlineStr">
+      <c r="L233" s="20" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="234">
-      <c r="A234" s="12" t="inlineStr">
+      <c r="A234" s="20" t="inlineStr">
         <is>
           <t>M065</t>
         </is>
       </c>
-      <c r="B234" s="13" t="inlineStr">
+      <c r="B234" s="21" t="inlineStr">
         <is>
           <t>Narration Match
 Lender Amount: 20733.00
 Borrower Amount: 20733.00</t>
         </is>
       </c>
-      <c r="C234" s="12" t="inlineStr"/>
-      <c r="D234" s="12" t="inlineStr"/>
-      <c r="E234" s="18" t="inlineStr">
+      <c r="C234" s="20" t="inlineStr"/>
+      <c r="D234" s="20" t="inlineStr"/>
+      <c r="E234" s="26" t="inlineStr">
         <is>
           <t>Salary of Pole unit paid to Steel unit for the month of June-2025.</t>
         </is>
       </c>
-      <c r="F234" s="12" t="inlineStr"/>
-      <c r="G234" s="12" t="inlineStr"/>
-      <c r="H234" s="12" t="inlineStr"/>
-      <c r="I234" s="12" t="inlineStr"/>
-      <c r="J234" s="12" t="inlineStr"/>
-      <c r="K234" s="12" t="inlineStr"/>
-      <c r="L234" s="12" t="inlineStr">
+      <c r="F234" s="20" t="inlineStr"/>
+      <c r="G234" s="20" t="inlineStr"/>
+      <c r="H234" s="20" t="inlineStr"/>
+      <c r="I234" s="20" t="inlineStr"/>
+      <c r="J234" s="20" t="inlineStr"/>
+      <c r="K234" s="20" t="inlineStr"/>
+      <c r="L234" s="20" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="235">
-      <c r="A235" s="12" t="inlineStr">
+      <c r="A235" s="20" t="inlineStr">
         <is>
           <t>M065</t>
         </is>
       </c>
-      <c r="B235" s="13" t="inlineStr"/>
-      <c r="C235" s="12" t="inlineStr"/>
-      <c r="D235" s="12" t="inlineStr">
+      <c r="B235" s="21" t="inlineStr"/>
+      <c r="C235" s="20" t="inlineStr"/>
+      <c r="D235" s="20" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E235" s="19" t="inlineStr">
+      <c r="E235" s="27" t="inlineStr">
         <is>
           <t>sayeda</t>
         </is>
       </c>
-      <c r="F235" s="12" t="inlineStr"/>
-      <c r="G235" s="12" t="inlineStr"/>
-      <c r="H235" s="12" t="inlineStr"/>
-      <c r="I235" s="12" t="inlineStr"/>
-      <c r="J235" s="12" t="inlineStr"/>
-      <c r="K235" s="12" t="inlineStr"/>
-      <c r="L235" s="12" t="inlineStr">
+      <c r="F235" s="20" t="inlineStr"/>
+      <c r="G235" s="20" t="inlineStr"/>
+      <c r="H235" s="20" t="inlineStr"/>
+      <c r="I235" s="20" t="inlineStr"/>
+      <c r="J235" s="20" t="inlineStr"/>
+      <c r="K235" s="20" t="inlineStr"/>
+      <c r="L235" s="20" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>

</xml_diff>

<commit_message>
Match Summary tags fixed
</commit_message>
<xml_diff>
--- a/Resources/Steel-Pole/Steel Book POLE_MATCHED.xlsx
+++ b/Resources/Steel-Pole/Steel Book POLE_MATCHED.xlsx
@@ -965,301 +965,324 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr"/>
-      <c r="B17" s="2" t="inlineStr"/>
-      <c r="C17" s="6" t="inlineStr">
+      <c r="A17" s="20" t="inlineStr">
+        <is>
+          <t>M126</t>
+        </is>
+      </c>
+      <c r="B17" s="21" t="inlineStr"/>
+      <c r="C17" s="22" t="inlineStr">
         <is>
           <t>01/Jun/2025</t>
         </is>
       </c>
-      <c r="D17" s="1" t="inlineStr">
+      <c r="D17" s="20" t="inlineStr">
         <is>
           <t>Dr</t>
         </is>
       </c>
-      <c r="E17" s="7" t="inlineStr">
+      <c r="E17" s="23" t="inlineStr">
         <is>
           <t>Mutual Trust Bank Ltd-SND-002-0320004355</t>
         </is>
       </c>
-      <c r="F17" s="1" t="inlineStr"/>
-      <c r="G17" s="1" t="inlineStr"/>
-      <c r="H17" s="9" t="inlineStr">
+      <c r="F17" s="20" t="inlineStr"/>
+      <c r="G17" s="20" t="inlineStr"/>
+      <c r="H17" s="24" t="inlineStr">
         <is>
           <t>Receipt</t>
         </is>
       </c>
-      <c r="I17" s="1" t="inlineStr">
+      <c r="I17" s="20" t="inlineStr">
         <is>
           <t>915</t>
         </is>
       </c>
-      <c r="J17" s="1" t="inlineStr"/>
-      <c r="K17" s="8" t="inlineStr">
+      <c r="J17" s="20" t="inlineStr"/>
+      <c r="K17" s="25" t="inlineStr">
         <is>
           <t>905515</t>
         </is>
       </c>
-      <c r="L17" s="1" t="inlineStr"/>
+      <c r="L17" s="20" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr"/>
-      <c r="B18" s="2" t="inlineStr">
-        <is>
-          <t>Unmatched Record
-Reasons:
-1. No interunit account found in File 2 block
-2. Settlement mismatch: File 1 IDs ['94976'], File 2 IDs []</t>
-        </is>
-      </c>
-      <c r="C18" s="1" t="inlineStr"/>
-      <c r="D18" s="1" t="inlineStr"/>
-      <c r="E18" s="10" t="inlineStr">
+      <c r="A18" s="20" t="inlineStr">
+        <is>
+          <t>M126</t>
+        </is>
+      </c>
+      <c r="B18" s="21" t="inlineStr">
+        <is>
+          <t>Manual Match
+Lender Amount: 905515.00
+Borrower Amount: 905515.00</t>
+        </is>
+      </c>
+      <c r="C18" s="20" t="inlineStr"/>
+      <c r="D18" s="20" t="inlineStr"/>
+      <c r="E18" s="26" t="inlineStr">
         <is>
           <t>Reversing....     Bank Payment date was 26.12.2024</t>
         </is>
       </c>
-      <c r="F18" s="1" t="inlineStr"/>
-      <c r="G18" s="1" t="inlineStr"/>
-      <c r="H18" s="1" t="inlineStr"/>
-      <c r="I18" s="1" t="inlineStr"/>
-      <c r="J18" s="1" t="inlineStr"/>
-      <c r="K18" s="1" t="inlineStr"/>
-      <c r="L18" s="1" t="inlineStr"/>
+      <c r="F18" s="20" t="inlineStr"/>
+      <c r="G18" s="20" t="inlineStr"/>
+      <c r="H18" s="20" t="inlineStr"/>
+      <c r="I18" s="20" t="inlineStr"/>
+      <c r="J18" s="20" t="inlineStr"/>
+      <c r="K18" s="20" t="inlineStr"/>
+      <c r="L18" s="20" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr"/>
-      <c r="B19" s="2" t="inlineStr"/>
-      <c r="C19" s="1" t="inlineStr"/>
-      <c r="D19" s="1" t="inlineStr">
+      <c r="A19" s="20" t="inlineStr">
+        <is>
+          <t>M126</t>
+        </is>
+      </c>
+      <c r="B19" s="21" t="inlineStr"/>
+      <c r="C19" s="20" t="inlineStr"/>
+      <c r="D19" s="20" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E19" s="11" t="inlineStr">
+      <c r="E19" s="27" t="inlineStr">
         <is>
           <t>g.azam</t>
         </is>
       </c>
-      <c r="F19" s="1" t="inlineStr"/>
-      <c r="G19" s="1" t="inlineStr"/>
-      <c r="H19" s="1" t="inlineStr"/>
-      <c r="I19" s="1" t="inlineStr"/>
-      <c r="J19" s="1" t="inlineStr"/>
-      <c r="K19" s="1" t="inlineStr"/>
-      <c r="L19" s="1" t="inlineStr"/>
+      <c r="F19" s="20" t="inlineStr"/>
+      <c r="G19" s="20" t="inlineStr"/>
+      <c r="H19" s="20" t="inlineStr"/>
+      <c r="I19" s="20" t="inlineStr"/>
+      <c r="J19" s="20" t="inlineStr"/>
+      <c r="K19" s="20" t="inlineStr"/>
+      <c r="L19" s="20" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="20" t="inlineStr">
+      <c r="A20" s="12" t="inlineStr">
         <is>
           <t>M122</t>
         </is>
       </c>
-      <c r="B20" s="21" t="inlineStr"/>
-      <c r="C20" s="22" t="inlineStr">
+      <c r="B20" s="13" t="inlineStr"/>
+      <c r="C20" s="14" t="inlineStr">
         <is>
           <t>02/Jun/2025</t>
         </is>
       </c>
-      <c r="D20" s="20" t="inlineStr">
+      <c r="D20" s="12" t="inlineStr">
         <is>
           <t>Dr</t>
         </is>
       </c>
-      <c r="E20" s="23" t="inlineStr">
+      <c r="E20" s="15" t="inlineStr">
         <is>
           <t>Eastern Bank PLC-OD-A/C-1012040000125</t>
         </is>
       </c>
-      <c r="F20" s="20" t="inlineStr"/>
-      <c r="G20" s="20" t="inlineStr"/>
-      <c r="H20" s="24" t="inlineStr">
+      <c r="F20" s="12" t="inlineStr"/>
+      <c r="G20" s="12" t="inlineStr"/>
+      <c r="H20" s="16" t="inlineStr">
         <is>
           <t>Receipt</t>
         </is>
       </c>
-      <c r="I20" s="20" t="inlineStr">
+      <c r="I20" s="12" t="inlineStr">
         <is>
           <t>927</t>
         </is>
       </c>
-      <c r="J20" s="20" t="inlineStr"/>
-      <c r="K20" s="25" t="inlineStr">
+      <c r="J20" s="12" t="inlineStr"/>
+      <c r="K20" s="17" t="inlineStr">
         <is>
           <t>18027176.54</t>
         </is>
       </c>
-      <c r="L20" s="20" t="inlineStr">
+      <c r="L20" s="12" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="20" t="inlineStr">
+      <c r="A21" s="12" t="inlineStr">
         <is>
           <t>M122</t>
         </is>
       </c>
-      <c r="B21" s="21" t="inlineStr">
+      <c r="B21" s="13" t="inlineStr">
         <is>
           <t>USD Match: $147,401.28
 Lender Amount: 18027176.54
 Borrower Amount: 18027176.54</t>
         </is>
       </c>
-      <c r="C21" s="20" t="inlineStr"/>
-      <c r="D21" s="20" t="inlineStr"/>
-      <c r="E21" s="26" t="inlineStr">
+      <c r="C21" s="12" t="inlineStr"/>
+      <c r="D21" s="12" t="inlineStr"/>
+      <c r="E21" s="18" t="inlineStr">
         <is>
           <t>Received Voucher: Amounts received agt PO number : MCEP/BREB/DMD-SPC-G-24-Lot-1/2023-2024-Part-1-WB, remark: Total Bill- 226851.20 usd. CIL Bill- Part1- 193819.20 usd+ Part2- 33032 usd) Total received- 226771.20 (Part1- 193819.20 usd+ Part2- 32952 usd). Bank charge -80 Usd.,  $147,401.28 @ Tk.122.30/-</t>
         </is>
       </c>
-      <c r="F21" s="20" t="inlineStr"/>
-      <c r="G21" s="20" t="inlineStr"/>
-      <c r="H21" s="20" t="inlineStr"/>
-      <c r="I21" s="20" t="inlineStr"/>
-      <c r="J21" s="20" t="inlineStr"/>
-      <c r="K21" s="20" t="inlineStr"/>
-      <c r="L21" s="20" t="inlineStr">
+      <c r="F21" s="12" t="inlineStr"/>
+      <c r="G21" s="12" t="inlineStr"/>
+      <c r="H21" s="12" t="inlineStr"/>
+      <c r="I21" s="12" t="inlineStr"/>
+      <c r="J21" s="12" t="inlineStr"/>
+      <c r="K21" s="12" t="inlineStr"/>
+      <c r="L21" s="12" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="20" t="inlineStr">
+      <c r="A22" s="12" t="inlineStr">
         <is>
           <t>M122</t>
         </is>
       </c>
-      <c r="B22" s="21" t="inlineStr"/>
-      <c r="C22" s="20" t="inlineStr"/>
-      <c r="D22" s="20" t="inlineStr">
+      <c r="B22" s="13" t="inlineStr"/>
+      <c r="C22" s="12" t="inlineStr"/>
+      <c r="D22" s="12" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E22" s="27" t="inlineStr">
+      <c r="E22" s="19" t="inlineStr">
         <is>
           <t>ashiq</t>
         </is>
       </c>
-      <c r="F22" s="20" t="inlineStr"/>
-      <c r="G22" s="20" t="inlineStr"/>
-      <c r="H22" s="20" t="inlineStr"/>
-      <c r="I22" s="20" t="inlineStr"/>
-      <c r="J22" s="20" t="inlineStr"/>
-      <c r="K22" s="20" t="inlineStr"/>
-      <c r="L22" s="20" t="inlineStr">
+      <c r="F22" s="12" t="inlineStr"/>
+      <c r="G22" s="12" t="inlineStr"/>
+      <c r="H22" s="12" t="inlineStr"/>
+      <c r="I22" s="12" t="inlineStr"/>
+      <c r="J22" s="12" t="inlineStr"/>
+      <c r="K22" s="12" t="inlineStr"/>
+      <c r="L22" s="12" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="12" t="inlineStr">
+      <c r="A23" s="20" t="inlineStr">
         <is>
           <t>M073</t>
         </is>
       </c>
-      <c r="B23" s="13" t="inlineStr"/>
-      <c r="C23" s="14" t="inlineStr">
+      <c r="B23" s="21" t="inlineStr"/>
+      <c r="C23" s="22" t="inlineStr">
         <is>
           <t>03/Jun/2025</t>
         </is>
       </c>
-      <c r="D23" s="12" t="inlineStr">
+      <c r="D23" s="20" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E23" s="15" t="inlineStr">
+      <c r="E23" s="23" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F23" s="12" t="inlineStr"/>
-      <c r="G23" s="12" t="inlineStr"/>
-      <c r="H23" s="16" t="inlineStr">
+      <c r="F23" s="20" t="inlineStr"/>
+      <c r="G23" s="20" t="inlineStr"/>
+      <c r="H23" s="24" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I23" s="12" t="inlineStr">
+      <c r="I23" s="20" t="inlineStr">
         <is>
           <t>70391</t>
         </is>
       </c>
-      <c r="J23" s="17" t="inlineStr">
+      <c r="J23" s="25" t="inlineStr">
         <is>
           <t>600000</t>
         </is>
       </c>
-      <c r="K23" s="12" t="inlineStr"/>
-      <c r="L23" s="12" t="inlineStr">
+      <c r="K23" s="20" t="inlineStr"/>
+      <c r="L23" s="20" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="12" t="inlineStr">
+      <c r="A24" s="20" t="inlineStr">
         <is>
           <t>M073</t>
         </is>
       </c>
-      <c r="B24" s="13" t="inlineStr">
+      <c r="B24" s="21" t="inlineStr">
         <is>
           <t>Interunit Loan Match: MDB#0331
 Lender Amount: 600000.00
 Borrower Amount: 600000.00</t>
         </is>
       </c>
-      <c r="C24" s="12" t="inlineStr"/>
-      <c r="D24" s="12" t="inlineStr"/>
-      <c r="E24" s="18" t="inlineStr">
+      <c r="C24" s="20" t="inlineStr"/>
+      <c r="D24" s="20" t="inlineStr"/>
+      <c r="E24" s="26" t="inlineStr">
         <is>
           <t>Being the amount paid to M/S. Mukta Engineering Works . Supply of , Invoice Number:  005, Challan Number: 005, Work Order Number: PBS/PO/2024/8/29211, BA Team (A), Company Unit: Concrete Pole &amp; Pile, Project Name : PBSF-G-260 (ID:949763), Work Order date: 2024-08-30, Goods Received Date: 2024-12-04, Work Order Value: 853990.0, Total Bill Amount: 797190.0, TDS Deduction Amount: 0.0, VDS Deduction Amount: 0.0</t>
         </is>
       </c>
-      <c r="F24" s="12" t="inlineStr"/>
-      <c r="G24" s="12" t="inlineStr"/>
-      <c r="H24" s="12" t="inlineStr"/>
-      <c r="I24" s="12" t="inlineStr"/>
-      <c r="J24" s="12" t="inlineStr"/>
-      <c r="K24" s="12" t="inlineStr"/>
-      <c r="L24" s="12" t="inlineStr">
+      <c r="F24" s="20" t="inlineStr"/>
+      <c r="G24" s="20" t="inlineStr"/>
+      <c r="H24" s="20" t="inlineStr"/>
+      <c r="I24" s="20" t="inlineStr"/>
+      <c r="J24" s="20" t="inlineStr"/>
+      <c r="K24" s="20" t="inlineStr"/>
+      <c r="L24" s="20" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="12" t="inlineStr">
+      <c r="A25" s="20" t="inlineStr">
         <is>
           <t>M073</t>
         </is>
       </c>
-      <c r="B25" s="13" t="inlineStr"/>
-      <c r="C25" s="12" t="inlineStr"/>
-      <c r="D25" s="12" t="inlineStr">
+      <c r="B25" s="21" t="inlineStr"/>
+      <c r="C25" s="20" t="inlineStr"/>
+      <c r="D25" s="20" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E25" s="19" t="inlineStr">
+      <c r="E25" s="27" t="inlineStr">
         <is>
           <t>ziaul</t>
         </is>
       </c>
-      <c r="F25" s="12" t="inlineStr"/>
-      <c r="G25" s="12" t="inlineStr"/>
-      <c r="H25" s="12" t="inlineStr"/>
-      <c r="I25" s="12" t="inlineStr"/>
-      <c r="J25" s="12" t="inlineStr"/>
-      <c r="K25" s="12" t="inlineStr"/>
-      <c r="L25" s="12" t="inlineStr">
+      <c r="F25" s="20" t="inlineStr"/>
+      <c r="G25" s="20" t="inlineStr"/>
+      <c r="H25" s="20" t="inlineStr"/>
+      <c r="I25" s="20" t="inlineStr"/>
+      <c r="J25" s="20" t="inlineStr"/>
+      <c r="K25" s="20" t="inlineStr"/>
+      <c r="L25" s="20" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
@@ -1440,433 +1463,433 @@
       <c r="L28" s="1" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" s="20" t="inlineStr">
+      <c r="A29" s="12" t="inlineStr">
         <is>
           <t>M077</t>
         </is>
       </c>
-      <c r="B29" s="21" t="inlineStr"/>
-      <c r="C29" s="22" t="inlineStr">
+      <c r="B29" s="13" t="inlineStr"/>
+      <c r="C29" s="14" t="inlineStr">
         <is>
           <t>03/Jun/2025</t>
         </is>
       </c>
-      <c r="D29" s="20" t="inlineStr">
+      <c r="D29" s="12" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E29" s="23" t="inlineStr">
+      <c r="E29" s="15" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F29" s="20" t="inlineStr"/>
-      <c r="G29" s="20" t="inlineStr"/>
-      <c r="H29" s="24" t="inlineStr">
+      <c r="F29" s="12" t="inlineStr"/>
+      <c r="G29" s="12" t="inlineStr"/>
+      <c r="H29" s="16" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I29" s="20" t="inlineStr">
+      <c r="I29" s="12" t="inlineStr">
         <is>
           <t>70394</t>
         </is>
       </c>
-      <c r="J29" s="25" t="inlineStr">
+      <c r="J29" s="17" t="inlineStr">
         <is>
           <t>700000</t>
         </is>
       </c>
-      <c r="K29" s="20" t="inlineStr"/>
-      <c r="L29" s="20" t="inlineStr">
+      <c r="K29" s="12" t="inlineStr"/>
+      <c r="L29" s="12" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="20" t="inlineStr">
+      <c r="A30" s="12" t="inlineStr">
         <is>
           <t>M077</t>
         </is>
       </c>
-      <c r="B30" s="21" t="inlineStr">
+      <c r="B30" s="13" t="inlineStr">
         <is>
           <t>Interunit Loan Match: MDB#0331
 Lender Amount: 700000.00
 Borrower Amount: 700000.00</t>
         </is>
       </c>
-      <c r="C30" s="20" t="inlineStr"/>
-      <c r="D30" s="20" t="inlineStr"/>
-      <c r="E30" s="26" t="inlineStr">
+      <c r="C30" s="12" t="inlineStr"/>
+      <c r="D30" s="12" t="inlineStr"/>
+      <c r="E30" s="18" t="inlineStr">
         <is>
           <t>Being the amount paid to Akij Cement Company Ltd.. Supply of , Invoice Number:  NOV24-14 (Bag), Challan Number: DC01020247652,DC01020246583, DC01020246584,DC01020247653, DC01020247654, Work Order Number: G24/PO/2024/9/29253, BA Team (A), Company Unit: Concrete Pole &amp; Pile, Project Name : WD1: LOT-1; MCEP/BREB/DMD SPC-G-24, Lot-1, Work Order date: 2024-09-03, Goods Received Date: 2024-11-05, Work Order Value: 5400000.0, Total Bill Amount: 873603.36, TDS Deduction Amount: 17828.64, VDS Deduction Amount: 0.0</t>
         </is>
       </c>
-      <c r="F30" s="20" t="inlineStr"/>
-      <c r="G30" s="20" t="inlineStr"/>
-      <c r="H30" s="20" t="inlineStr"/>
-      <c r="I30" s="20" t="inlineStr"/>
-      <c r="J30" s="20" t="inlineStr"/>
-      <c r="K30" s="20" t="inlineStr"/>
-      <c r="L30" s="20" t="inlineStr">
+      <c r="F30" s="12" t="inlineStr"/>
+      <c r="G30" s="12" t="inlineStr"/>
+      <c r="H30" s="12" t="inlineStr"/>
+      <c r="I30" s="12" t="inlineStr"/>
+      <c r="J30" s="12" t="inlineStr"/>
+      <c r="K30" s="12" t="inlineStr"/>
+      <c r="L30" s="12" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="20" t="inlineStr">
+      <c r="A31" s="12" t="inlineStr">
         <is>
           <t>M077</t>
         </is>
       </c>
-      <c r="B31" s="21" t="inlineStr"/>
-      <c r="C31" s="20" t="inlineStr"/>
-      <c r="D31" s="20" t="inlineStr">
+      <c r="B31" s="13" t="inlineStr"/>
+      <c r="C31" s="12" t="inlineStr"/>
+      <c r="D31" s="12" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E31" s="27" t="inlineStr">
+      <c r="E31" s="19" t="inlineStr">
         <is>
           <t>ziaul</t>
         </is>
       </c>
-      <c r="F31" s="20" t="inlineStr"/>
-      <c r="G31" s="20" t="inlineStr"/>
-      <c r="H31" s="20" t="inlineStr"/>
-      <c r="I31" s="20" t="inlineStr"/>
-      <c r="J31" s="20" t="inlineStr"/>
-      <c r="K31" s="20" t="inlineStr"/>
-      <c r="L31" s="20" t="inlineStr">
+      <c r="F31" s="12" t="inlineStr"/>
+      <c r="G31" s="12" t="inlineStr"/>
+      <c r="H31" s="12" t="inlineStr"/>
+      <c r="I31" s="12" t="inlineStr"/>
+      <c r="J31" s="12" t="inlineStr"/>
+      <c r="K31" s="12" t="inlineStr"/>
+      <c r="L31" s="12" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="12" t="inlineStr">
+      <c r="A32" s="20" t="inlineStr">
         <is>
           <t>M001</t>
         </is>
       </c>
-      <c r="B32" s="13" t="inlineStr"/>
-      <c r="C32" s="14" t="inlineStr">
+      <c r="B32" s="21" t="inlineStr"/>
+      <c r="C32" s="22" t="inlineStr">
         <is>
           <t>03/Jun/2025</t>
         </is>
       </c>
-      <c r="D32" s="12" t="inlineStr">
+      <c r="D32" s="20" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E32" s="15" t="inlineStr">
+      <c r="E32" s="23" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F32" s="12" t="inlineStr"/>
-      <c r="G32" s="12" t="inlineStr"/>
-      <c r="H32" s="16" t="inlineStr">
+      <c r="F32" s="20" t="inlineStr"/>
+      <c r="G32" s="20" t="inlineStr"/>
+      <c r="H32" s="24" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I32" s="12" t="inlineStr">
+      <c r="I32" s="20" t="inlineStr">
         <is>
           <t>70395</t>
         </is>
       </c>
-      <c r="J32" s="17" t="inlineStr">
+      <c r="J32" s="25" t="inlineStr">
         <is>
           <t>300000</t>
         </is>
       </c>
-      <c r="K32" s="12" t="inlineStr"/>
-      <c r="L32" s="12" t="inlineStr">
+      <c r="K32" s="20" t="inlineStr"/>
+      <c r="L32" s="20" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="12" t="inlineStr">
+      <c r="A33" s="20" t="inlineStr">
         <is>
           <t>M001</t>
         </is>
       </c>
-      <c r="B33" s="13" t="inlineStr">
+      <c r="B33" s="21" t="inlineStr">
         <is>
           <t>PO Match: DMD/PO/2024/12/31413
 Lender Amount: 300000.00
 Borrower Amount: 300000.00</t>
         </is>
       </c>
-      <c r="C33" s="12" t="inlineStr"/>
-      <c r="D33" s="12" t="inlineStr"/>
-      <c r="E33" s="18" t="inlineStr">
+      <c r="C33" s="20" t="inlineStr"/>
+      <c r="D33" s="20" t="inlineStr"/>
+      <c r="E33" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve">Being the amount paid to M/S. Alif  Enterprise. Supply of , Invoice Number:  214, Challan Number: 011,012,013,015,005,007,008,009,010.,014, 016, 017,020, Work Order Number: DMD/PO/2024/12/31413, BA Team (A), Company Unit: Concrete Pole &amp; Pile, Project Name : DMD-SPC-G-24-Lot-1-Part-2-WB, Work Order date: 2024-12-30, Goods Received Date: 2025-01-18,2025-01-11,2025-01-30, Work Order Value: 1104000.0, Total Bill Amount: 300000.0, TDS Deduction Amount: 0.0, VDS Deduction Amount: 0.0  P-58272_x000D_
 </t>
         </is>
       </c>
-      <c r="F33" s="12" t="inlineStr"/>
-      <c r="G33" s="12" t="inlineStr"/>
-      <c r="H33" s="12" t="inlineStr"/>
-      <c r="I33" s="12" t="inlineStr"/>
-      <c r="J33" s="12" t="inlineStr"/>
-      <c r="K33" s="12" t="inlineStr"/>
-      <c r="L33" s="12" t="inlineStr">
+      <c r="F33" s="20" t="inlineStr"/>
+      <c r="G33" s="20" t="inlineStr"/>
+      <c r="H33" s="20" t="inlineStr"/>
+      <c r="I33" s="20" t="inlineStr"/>
+      <c r="J33" s="20" t="inlineStr"/>
+      <c r="K33" s="20" t="inlineStr"/>
+      <c r="L33" s="20" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="12" t="inlineStr">
+      <c r="A34" s="20" t="inlineStr">
         <is>
           <t>M001</t>
         </is>
       </c>
-      <c r="B34" s="13" t="inlineStr"/>
-      <c r="C34" s="12" t="inlineStr"/>
-      <c r="D34" s="12" t="inlineStr">
+      <c r="B34" s="21" t="inlineStr"/>
+      <c r="C34" s="20" t="inlineStr"/>
+      <c r="D34" s="20" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E34" s="19" t="inlineStr">
+      <c r="E34" s="27" t="inlineStr">
         <is>
           <t>mahbub.alam</t>
         </is>
       </c>
-      <c r="F34" s="12" t="inlineStr"/>
-      <c r="G34" s="12" t="inlineStr"/>
-      <c r="H34" s="12" t="inlineStr"/>
-      <c r="I34" s="12" t="inlineStr"/>
-      <c r="J34" s="12" t="inlineStr"/>
-      <c r="K34" s="12" t="inlineStr"/>
-      <c r="L34" s="12" t="inlineStr">
+      <c r="F34" s="20" t="inlineStr"/>
+      <c r="G34" s="20" t="inlineStr"/>
+      <c r="H34" s="20" t="inlineStr"/>
+      <c r="I34" s="20" t="inlineStr"/>
+      <c r="J34" s="20" t="inlineStr"/>
+      <c r="K34" s="20" t="inlineStr"/>
+      <c r="L34" s="20" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="20" t="inlineStr">
+      <c r="A35" s="12" t="inlineStr">
         <is>
           <t>M075</t>
         </is>
       </c>
-      <c r="B35" s="21" t="inlineStr"/>
-      <c r="C35" s="22" t="inlineStr">
+      <c r="B35" s="13" t="inlineStr"/>
+      <c r="C35" s="14" t="inlineStr">
         <is>
           <t>03/Jun/2025</t>
         </is>
       </c>
-      <c r="D35" s="20" t="inlineStr">
+      <c r="D35" s="12" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E35" s="23" t="inlineStr">
+      <c r="E35" s="15" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F35" s="20" t="inlineStr"/>
-      <c r="G35" s="20" t="inlineStr"/>
-      <c r="H35" s="24" t="inlineStr">
+      <c r="F35" s="12" t="inlineStr"/>
+      <c r="G35" s="12" t="inlineStr"/>
+      <c r="H35" s="16" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I35" s="20" t="inlineStr">
+      <c r="I35" s="12" t="inlineStr">
         <is>
           <t>70396</t>
         </is>
       </c>
-      <c r="J35" s="25" t="inlineStr">
+      <c r="J35" s="17" t="inlineStr">
         <is>
           <t>700000</t>
         </is>
       </c>
-      <c r="K35" s="20" t="inlineStr"/>
-      <c r="L35" s="20" t="inlineStr">
+      <c r="K35" s="12" t="inlineStr"/>
+      <c r="L35" s="12" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="20" t="inlineStr">
+      <c r="A36" s="12" t="inlineStr">
         <is>
           <t>M075</t>
         </is>
       </c>
-      <c r="B36" s="21" t="inlineStr">
+      <c r="B36" s="13" t="inlineStr">
         <is>
           <t>Interunit Loan Match: MDB#0331
 Lender Amount: 700000.00
 Borrower Amount: 700000.00</t>
         </is>
       </c>
-      <c r="C36" s="20" t="inlineStr"/>
-      <c r="D36" s="20" t="inlineStr"/>
-      <c r="E36" s="26" t="inlineStr">
+      <c r="C36" s="12" t="inlineStr"/>
+      <c r="D36" s="12" t="inlineStr"/>
+      <c r="E36" s="18" t="inlineStr">
         <is>
           <t>Being the amount paid to Crown Cement PLC. Supply of , Invoice Number:  147, Challan Number: 8002103646, 8002103650,8002107843, 8002107850,8002103872, 8002103674,8002112659, 8002112833, 8002112835, 8002112911, 8002112961,,8002116901, 8002116920,8002121931,8002107848, Work Order Number: PBS/PO/2024/11/30298, BA Team (A), Company Unit: Concrete Pole &amp; Pile, Project Name : PBSF-G-260 (ID:949763), Work Order date: 2024-11-07, Goods Received Date: 2024-11-21,2024-11-28,2024-12-05,2024-12-02, Work Order Value: 3120000.0, Total Bill Amount: 2777895.84, TDS Deduction Amount: 56691.75, VDS Deduction Amount: 0.0</t>
         </is>
       </c>
-      <c r="F36" s="20" t="inlineStr"/>
-      <c r="G36" s="20" t="inlineStr"/>
-      <c r="H36" s="20" t="inlineStr"/>
-      <c r="I36" s="20" t="inlineStr"/>
-      <c r="J36" s="20" t="inlineStr"/>
-      <c r="K36" s="20" t="inlineStr"/>
-      <c r="L36" s="20" t="inlineStr">
+      <c r="F36" s="12" t="inlineStr"/>
+      <c r="G36" s="12" t="inlineStr"/>
+      <c r="H36" s="12" t="inlineStr"/>
+      <c r="I36" s="12" t="inlineStr"/>
+      <c r="J36" s="12" t="inlineStr"/>
+      <c r="K36" s="12" t="inlineStr"/>
+      <c r="L36" s="12" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="20" t="inlineStr">
+      <c r="A37" s="12" t="inlineStr">
         <is>
           <t>M075</t>
         </is>
       </c>
-      <c r="B37" s="21" t="inlineStr"/>
-      <c r="C37" s="20" t="inlineStr"/>
-      <c r="D37" s="20" t="inlineStr">
+      <c r="B37" s="13" t="inlineStr"/>
+      <c r="C37" s="12" t="inlineStr"/>
+      <c r="D37" s="12" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E37" s="27" t="inlineStr">
+      <c r="E37" s="19" t="inlineStr">
         <is>
           <t>ziaul</t>
         </is>
       </c>
-      <c r="F37" s="20" t="inlineStr"/>
-      <c r="G37" s="20" t="inlineStr"/>
-      <c r="H37" s="20" t="inlineStr"/>
-      <c r="I37" s="20" t="inlineStr"/>
-      <c r="J37" s="20" t="inlineStr"/>
-      <c r="K37" s="20" t="inlineStr"/>
-      <c r="L37" s="20" t="inlineStr">
+      <c r="F37" s="12" t="inlineStr"/>
+      <c r="G37" s="12" t="inlineStr"/>
+      <c r="H37" s="12" t="inlineStr"/>
+      <c r="I37" s="12" t="inlineStr"/>
+      <c r="J37" s="12" t="inlineStr"/>
+      <c r="K37" s="12" t="inlineStr"/>
+      <c r="L37" s="12" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="12" t="inlineStr">
+      <c r="A38" s="20" t="inlineStr">
         <is>
           <t>M076</t>
         </is>
       </c>
-      <c r="B38" s="13" t="inlineStr"/>
-      <c r="C38" s="14" t="inlineStr">
+      <c r="B38" s="21" t="inlineStr"/>
+      <c r="C38" s="22" t="inlineStr">
         <is>
           <t>03/Jun/2025</t>
         </is>
       </c>
-      <c r="D38" s="12" t="inlineStr">
+      <c r="D38" s="20" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E38" s="15" t="inlineStr">
+      <c r="E38" s="23" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F38" s="12" t="inlineStr"/>
-      <c r="G38" s="12" t="inlineStr"/>
-      <c r="H38" s="16" t="inlineStr">
+      <c r="F38" s="20" t="inlineStr"/>
+      <c r="G38" s="20" t="inlineStr"/>
+      <c r="H38" s="24" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I38" s="12" t="inlineStr">
+      <c r="I38" s="20" t="inlineStr">
         <is>
           <t>70397</t>
         </is>
       </c>
-      <c r="J38" s="17" t="inlineStr">
+      <c r="J38" s="25" t="inlineStr">
         <is>
           <t>100000</t>
         </is>
       </c>
-      <c r="K38" s="12" t="inlineStr"/>
-      <c r="L38" s="12" t="inlineStr">
+      <c r="K38" s="20" t="inlineStr"/>
+      <c r="L38" s="20" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="12" t="inlineStr">
+      <c r="A39" s="20" t="inlineStr">
         <is>
           <t>M076</t>
         </is>
       </c>
-      <c r="B39" s="13" t="inlineStr">
+      <c r="B39" s="21" t="inlineStr">
         <is>
           <t>Interunit Loan Match: MDB#0331
 Lender Amount: 100000.00
 Borrower Amount: 100000.00</t>
         </is>
       </c>
-      <c r="C39" s="12" t="inlineStr"/>
-      <c r="D39" s="12" t="inlineStr"/>
-      <c r="E39" s="18" t="inlineStr">
+      <c r="C39" s="20" t="inlineStr"/>
+      <c r="D39" s="20" t="inlineStr"/>
+      <c r="E39" s="26" t="inlineStr">
         <is>
           <t>Being the amount paid to BSRM Wires Limited. Supply of , Invoice Number:  424001088, Challan Number: 3060537, Work Order Number: DES/PO/2024/11/30582, BA Team (A), Company Unit: Concrete Pole &amp; Pile, Project Name : DESCO SPC Pole (GD-4), Work Order date: 2024-11-27, Goods Received Date: 2024-12-03, Work Order Value: 204668.0, Total Bill Amount: 199329.0, TDS Deduction Amount: 0.0, VDS Deduction Amount: 0.0</t>
         </is>
       </c>
-      <c r="F39" s="12" t="inlineStr"/>
-      <c r="G39" s="12" t="inlineStr"/>
-      <c r="H39" s="12" t="inlineStr"/>
-      <c r="I39" s="12" t="inlineStr"/>
-      <c r="J39" s="12" t="inlineStr"/>
-      <c r="K39" s="12" t="inlineStr"/>
-      <c r="L39" s="12" t="inlineStr">
+      <c r="F39" s="20" t="inlineStr"/>
+      <c r="G39" s="20" t="inlineStr"/>
+      <c r="H39" s="20" t="inlineStr"/>
+      <c r="I39" s="20" t="inlineStr"/>
+      <c r="J39" s="20" t="inlineStr"/>
+      <c r="K39" s="20" t="inlineStr"/>
+      <c r="L39" s="20" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="12" t="inlineStr">
+      <c r="A40" s="20" t="inlineStr">
         <is>
           <t>M076</t>
         </is>
       </c>
-      <c r="B40" s="13" t="inlineStr"/>
-      <c r="C40" s="12" t="inlineStr"/>
-      <c r="D40" s="12" t="inlineStr">
+      <c r="B40" s="21" t="inlineStr"/>
+      <c r="C40" s="20" t="inlineStr"/>
+      <c r="D40" s="20" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E40" s="19" t="inlineStr">
+      <c r="E40" s="27" t="inlineStr">
         <is>
           <t>ziaul</t>
         </is>
       </c>
-      <c r="F40" s="12" t="inlineStr"/>
-      <c r="G40" s="12" t="inlineStr"/>
-      <c r="H40" s="12" t="inlineStr"/>
-      <c r="I40" s="12" t="inlineStr"/>
-      <c r="J40" s="12" t="inlineStr"/>
-      <c r="K40" s="12" t="inlineStr"/>
-      <c r="L40" s="12" t="inlineStr">
+      <c r="F40" s="20" t="inlineStr"/>
+      <c r="G40" s="20" t="inlineStr"/>
+      <c r="H40" s="20" t="inlineStr"/>
+      <c r="I40" s="20" t="inlineStr"/>
+      <c r="J40" s="20" t="inlineStr"/>
+      <c r="K40" s="20" t="inlineStr"/>
+      <c r="L40" s="20" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
@@ -2181,691 +2204,760 @@
       <c r="L48" s="1" t="inlineStr"/>
     </row>
     <row r="49">
-      <c r="A49" s="20" t="inlineStr">
+      <c r="A49" s="12" t="inlineStr">
         <is>
           <t>M078</t>
         </is>
       </c>
-      <c r="B49" s="21" t="inlineStr"/>
-      <c r="C49" s="22" t="inlineStr">
+      <c r="B49" s="13" t="inlineStr"/>
+      <c r="C49" s="14" t="inlineStr">
         <is>
           <t>04/Jun/2025</t>
         </is>
       </c>
-      <c r="D49" s="20" t="inlineStr">
+      <c r="D49" s="12" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E49" s="23" t="inlineStr">
+      <c r="E49" s="15" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F49" s="20" t="inlineStr"/>
-      <c r="G49" s="20" t="inlineStr"/>
-      <c r="H49" s="24" t="inlineStr">
+      <c r="F49" s="12" t="inlineStr"/>
+      <c r="G49" s="12" t="inlineStr"/>
+      <c r="H49" s="16" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I49" s="20" t="inlineStr">
+      <c r="I49" s="12" t="inlineStr">
         <is>
           <t>70400</t>
         </is>
       </c>
-      <c r="J49" s="25" t="inlineStr">
+      <c r="J49" s="17" t="inlineStr">
         <is>
           <t>200000</t>
         </is>
       </c>
-      <c r="K49" s="20" t="inlineStr"/>
-      <c r="L49" s="20" t="inlineStr">
+      <c r="K49" s="12" t="inlineStr"/>
+      <c r="L49" s="12" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="20" t="inlineStr">
+      <c r="A50" s="12" t="inlineStr">
         <is>
           <t>M078</t>
         </is>
       </c>
-      <c r="B50" s="21" t="inlineStr">
+      <c r="B50" s="13" t="inlineStr">
         <is>
           <t>Interunit Loan Match: MDB#0331
 Lender Amount: 200000.00
 Borrower Amount: 200000.00</t>
         </is>
       </c>
-      <c r="C50" s="20" t="inlineStr"/>
-      <c r="D50" s="20" t="inlineStr"/>
-      <c r="E50" s="26" t="inlineStr">
+      <c r="C50" s="12" t="inlineStr"/>
+      <c r="D50" s="12" t="inlineStr"/>
+      <c r="E50" s="18" t="inlineStr">
         <is>
           <t>Being the amount paid to M/S. Sweet Enterprise. Supply of , Invoice Number:  053, Challan Number: 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757,1741, Work Order Number: PBS/PO/2024/10/29823, BA Team (A), Company Unit: Concrete Pole &amp; Pile, Project Name : PBSF-G-260 (ID:949763), Work Order date: 2024-10-03, Goods Received Date: 2024-10-12, Work Order Value: 1800000.0, Total Bill Amount: 703890.0, TDS Deduction Amount: 0.0, VDS Deduction Amount: 0.0</t>
         </is>
       </c>
-      <c r="F50" s="20" t="inlineStr"/>
-      <c r="G50" s="20" t="inlineStr"/>
-      <c r="H50" s="20" t="inlineStr"/>
-      <c r="I50" s="20" t="inlineStr"/>
-      <c r="J50" s="20" t="inlineStr"/>
-      <c r="K50" s="20" t="inlineStr"/>
-      <c r="L50" s="20" t="inlineStr">
+      <c r="F50" s="12" t="inlineStr"/>
+      <c r="G50" s="12" t="inlineStr"/>
+      <c r="H50" s="12" t="inlineStr"/>
+      <c r="I50" s="12" t="inlineStr"/>
+      <c r="J50" s="12" t="inlineStr"/>
+      <c r="K50" s="12" t="inlineStr"/>
+      <c r="L50" s="12" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="20" t="inlineStr">
+      <c r="A51" s="12" t="inlineStr">
         <is>
           <t>M078</t>
         </is>
       </c>
-      <c r="B51" s="21" t="inlineStr"/>
-      <c r="C51" s="20" t="inlineStr"/>
-      <c r="D51" s="20" t="inlineStr">
+      <c r="B51" s="13" t="inlineStr"/>
+      <c r="C51" s="12" t="inlineStr"/>
+      <c r="D51" s="12" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E51" s="27" t="inlineStr">
+      <c r="E51" s="19" t="inlineStr">
         <is>
           <t>ziaul</t>
         </is>
       </c>
-      <c r="F51" s="20" t="inlineStr"/>
-      <c r="G51" s="20" t="inlineStr"/>
-      <c r="H51" s="20" t="inlineStr"/>
-      <c r="I51" s="20" t="inlineStr"/>
-      <c r="J51" s="20" t="inlineStr"/>
-      <c r="K51" s="20" t="inlineStr"/>
-      <c r="L51" s="20" t="inlineStr">
+      <c r="F51" s="12" t="inlineStr"/>
+      <c r="G51" s="12" t="inlineStr"/>
+      <c r="H51" s="12" t="inlineStr"/>
+      <c r="I51" s="12" t="inlineStr"/>
+      <c r="J51" s="12" t="inlineStr"/>
+      <c r="K51" s="12" t="inlineStr"/>
+      <c r="L51" s="12" t="inlineStr">
         <is>
           <t>PO</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="12" t="inlineStr">
+      <c r="A52" s="20" t="inlineStr">
         <is>
           <t>M123</t>
         </is>
       </c>
-      <c r="B52" s="13" t="inlineStr"/>
-      <c r="C52" s="14" t="inlineStr">
+      <c r="B52" s="21" t="inlineStr"/>
+      <c r="C52" s="22" t="inlineStr">
         <is>
           <t>04/Jun/2025</t>
         </is>
       </c>
-      <c r="D52" s="12" t="inlineStr">
+      <c r="D52" s="20" t="inlineStr">
         <is>
           <t>Dr</t>
         </is>
       </c>
-      <c r="E52" s="15" t="inlineStr">
+      <c r="E52" s="23" t="inlineStr">
         <is>
           <t>Eastern Bank PLC-OD-A/C-1012040000125</t>
         </is>
       </c>
-      <c r="F52" s="12" t="inlineStr"/>
-      <c r="G52" s="12" t="inlineStr"/>
-      <c r="H52" s="16" t="inlineStr">
+      <c r="F52" s="20" t="inlineStr"/>
+      <c r="G52" s="20" t="inlineStr"/>
+      <c r="H52" s="24" t="inlineStr">
         <is>
           <t>Receipt</t>
         </is>
       </c>
-      <c r="I52" s="12" t="inlineStr">
+      <c r="I52" s="20" t="inlineStr">
         <is>
           <t>941</t>
         </is>
       </c>
-      <c r="J52" s="12" t="inlineStr"/>
-      <c r="K52" s="17" t="inlineStr">
+      <c r="J52" s="20" t="inlineStr"/>
+      <c r="K52" s="25" t="inlineStr">
         <is>
           <t>41625247.63</t>
         </is>
       </c>
-      <c r="L52" s="12" t="inlineStr">
+      <c r="L52" s="20" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="12" t="inlineStr">
+      <c r="A53" s="20" t="inlineStr">
         <is>
           <t>M123</t>
         </is>
       </c>
-      <c r="B53" s="13" t="inlineStr">
+      <c r="B53" s="21" t="inlineStr">
         <is>
           <t>USD Match: $.789,663.20
 Lender Amount: 41625247.63
 Borrower Amount: 41625247.63</t>
         </is>
       </c>
-      <c r="C53" s="12" t="inlineStr"/>
-      <c r="D53" s="12" t="inlineStr"/>
-      <c r="E53" s="18" t="inlineStr">
+      <c r="C53" s="20" t="inlineStr"/>
+      <c r="D53" s="20" t="inlineStr"/>
+      <c r="E53" s="26" t="inlineStr">
         <is>
           <t>Amount received agst Contract no.MCEP/BREB/DMD-SPC-G-24-Lot-1/2023-2024. Date.07.07.2024 This amount actually Pole Unit but deposit in Geo Textile Unit. Total bill amount $.789,663.20/- But ($.443,663.42+$6,400) Deposit in Geo Textile Unit. Remaining   $339520.78 Deposit in Steel Unit. Bank charge-$80. Rate.122.60</t>
         </is>
       </c>
-      <c r="F53" s="12" t="inlineStr"/>
-      <c r="G53" s="12" t="inlineStr"/>
-      <c r="H53" s="12" t="inlineStr"/>
-      <c r="I53" s="12" t="inlineStr"/>
-      <c r="J53" s="12" t="inlineStr"/>
-      <c r="K53" s="12" t="inlineStr"/>
-      <c r="L53" s="12" t="inlineStr">
+      <c r="F53" s="20" t="inlineStr"/>
+      <c r="G53" s="20" t="inlineStr"/>
+      <c r="H53" s="20" t="inlineStr"/>
+      <c r="I53" s="20" t="inlineStr"/>
+      <c r="J53" s="20" t="inlineStr"/>
+      <c r="K53" s="20" t="inlineStr"/>
+      <c r="L53" s="20" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="12" t="inlineStr">
+      <c r="A54" s="20" t="inlineStr">
         <is>
           <t>M123</t>
         </is>
       </c>
-      <c r="B54" s="13" t="inlineStr"/>
-      <c r="C54" s="12" t="inlineStr"/>
-      <c r="D54" s="12" t="inlineStr">
+      <c r="B54" s="21" t="inlineStr"/>
+      <c r="C54" s="20" t="inlineStr"/>
+      <c r="D54" s="20" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E54" s="19" t="inlineStr">
+      <c r="E54" s="27" t="inlineStr">
         <is>
           <t>sayeda</t>
         </is>
       </c>
-      <c r="F54" s="12" t="inlineStr"/>
-      <c r="G54" s="12" t="inlineStr"/>
-      <c r="H54" s="12" t="inlineStr"/>
-      <c r="I54" s="12" t="inlineStr"/>
-      <c r="J54" s="12" t="inlineStr"/>
-      <c r="K54" s="12" t="inlineStr"/>
-      <c r="L54" s="12" t="inlineStr">
+      <c r="F54" s="20" t="inlineStr"/>
+      <c r="G54" s="20" t="inlineStr"/>
+      <c r="H54" s="20" t="inlineStr"/>
+      <c r="I54" s="20" t="inlineStr"/>
+      <c r="J54" s="20" t="inlineStr"/>
+      <c r="K54" s="20" t="inlineStr"/>
+      <c r="L54" s="20" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="20" t="inlineStr">
+      <c r="A55" s="12" t="inlineStr">
         <is>
           <t>M002</t>
         </is>
       </c>
-      <c r="B55" s="21" t="inlineStr"/>
-      <c r="C55" s="22" t="inlineStr">
+      <c r="B55" s="13" t="inlineStr"/>
+      <c r="C55" s="14" t="inlineStr">
         <is>
           <t>04/Jun/2025</t>
         </is>
       </c>
-      <c r="D55" s="20" t="inlineStr">
+      <c r="D55" s="12" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E55" s="23" t="inlineStr">
+      <c r="E55" s="15" t="inlineStr">
         <is>
           <t>Mutual Trust Bank Ltd-SND-002-0320004355</t>
         </is>
       </c>
-      <c r="F55" s="20" t="inlineStr"/>
-      <c r="G55" s="20" t="inlineStr"/>
-      <c r="H55" s="24" t="inlineStr">
+      <c r="F55" s="12" t="inlineStr"/>
+      <c r="G55" s="12" t="inlineStr"/>
+      <c r="H55" s="16" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I55" s="20" t="inlineStr">
+      <c r="I55" s="12" t="inlineStr">
         <is>
           <t>70804</t>
         </is>
       </c>
-      <c r="J55" s="25" t="inlineStr">
+      <c r="J55" s="17" t="inlineStr">
         <is>
           <t>36600000</t>
         </is>
       </c>
-      <c r="K55" s="20" t="inlineStr"/>
-      <c r="L55" s="20" t="inlineStr">
+      <c r="K55" s="12" t="inlineStr"/>
+      <c r="L55" s="12" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="20" t="inlineStr">
+      <c r="A56" s="12" t="inlineStr">
         <is>
           <t>M002</t>
         </is>
       </c>
-      <c r="B56" s="21" t="inlineStr">
+      <c r="B56" s="13" t="inlineStr">
         <is>
           <t>USD Match: $300,000
 Lender Amount: 36600000.00
 Borrower Amount: 36600000.00</t>
         </is>
       </c>
-      <c r="C56" s="20" t="inlineStr"/>
-      <c r="D56" s="20" t="inlineStr"/>
-      <c r="E56" s="26" t="inlineStr">
+      <c r="C56" s="12" t="inlineStr"/>
+      <c r="D56" s="12" t="inlineStr"/>
+      <c r="E56" s="18" t="inlineStr">
         <is>
           <t>Amount pais to Sundry Party-Castle Construction Co.Ltd. $300,000 @ Tk.122/-</t>
         </is>
       </c>
-      <c r="F56" s="20" t="inlineStr"/>
-      <c r="G56" s="20" t="inlineStr"/>
-      <c r="H56" s="20" t="inlineStr"/>
-      <c r="I56" s="20" t="inlineStr"/>
-      <c r="J56" s="20" t="inlineStr"/>
-      <c r="K56" s="20" t="inlineStr"/>
-      <c r="L56" s="20" t="inlineStr">
+      <c r="F56" s="12" t="inlineStr"/>
+      <c r="G56" s="12" t="inlineStr"/>
+      <c r="H56" s="12" t="inlineStr"/>
+      <c r="I56" s="12" t="inlineStr"/>
+      <c r="J56" s="12" t="inlineStr"/>
+      <c r="K56" s="12" t="inlineStr"/>
+      <c r="L56" s="12" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="20" t="inlineStr">
+      <c r="A57" s="12" t="inlineStr">
         <is>
           <t>M002</t>
         </is>
       </c>
-      <c r="B57" s="21" t="inlineStr"/>
-      <c r="C57" s="20" t="inlineStr"/>
-      <c r="D57" s="20" t="inlineStr">
+      <c r="B57" s="13" t="inlineStr"/>
+      <c r="C57" s="12" t="inlineStr"/>
+      <c r="D57" s="12" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E57" s="27" t="inlineStr">
+      <c r="E57" s="19" t="inlineStr">
         <is>
           <t>ashiq</t>
         </is>
       </c>
-      <c r="F57" s="20" t="inlineStr"/>
-      <c r="G57" s="20" t="inlineStr"/>
-      <c r="H57" s="20" t="inlineStr"/>
-      <c r="I57" s="20" t="inlineStr"/>
-      <c r="J57" s="20" t="inlineStr"/>
-      <c r="K57" s="20" t="inlineStr"/>
-      <c r="L57" s="20" t="inlineStr">
+      <c r="F57" s="12" t="inlineStr"/>
+      <c r="G57" s="12" t="inlineStr"/>
+      <c r="H57" s="12" t="inlineStr"/>
+      <c r="I57" s="12" t="inlineStr"/>
+      <c r="J57" s="12" t="inlineStr"/>
+      <c r="K57" s="12" t="inlineStr"/>
+      <c r="L57" s="12" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="12" t="inlineStr">
+      <c r="A58" s="20" t="inlineStr">
         <is>
           <t>M004</t>
         </is>
       </c>
-      <c r="B58" s="13" t="inlineStr"/>
-      <c r="C58" s="14" t="inlineStr">
+      <c r="B58" s="21" t="inlineStr"/>
+      <c r="C58" s="22" t="inlineStr">
         <is>
           <t>05/Jun/2025</t>
         </is>
       </c>
-      <c r="D58" s="12" t="inlineStr">
+      <c r="D58" s="20" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E58" s="15" t="inlineStr">
+      <c r="E58" s="23" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F58" s="12" t="inlineStr"/>
-      <c r="G58" s="12" t="inlineStr"/>
-      <c r="H58" s="16" t="inlineStr">
+      <c r="F58" s="20" t="inlineStr"/>
+      <c r="G58" s="20" t="inlineStr"/>
+      <c r="H58" s="24" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I58" s="12" t="inlineStr">
+      <c r="I58" s="20" t="inlineStr">
         <is>
           <t>70845</t>
         </is>
       </c>
-      <c r="J58" s="17" t="inlineStr">
+      <c r="J58" s="25" t="inlineStr">
         <is>
           <t>62525</t>
         </is>
       </c>
-      <c r="K58" s="12" t="inlineStr"/>
-      <c r="L58" s="12" t="inlineStr">
+      <c r="K58" s="20" t="inlineStr"/>
+      <c r="L58" s="20" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="12" t="inlineStr">
+      <c r="A59" s="20" t="inlineStr">
         <is>
           <t>M004</t>
         </is>
       </c>
-      <c r="B59" s="13" t="inlineStr">
+      <c r="B59" s="21" t="inlineStr">
         <is>
           <t>Narration Match
 Lender Amount: 62525.00
 Borrower Amount: 62525.00</t>
         </is>
       </c>
-      <c r="C59" s="12" t="inlineStr"/>
-      <c r="D59" s="12" t="inlineStr"/>
-      <c r="E59" s="18" t="inlineStr">
+      <c r="C59" s="20" t="inlineStr"/>
+      <c r="D59" s="20" t="inlineStr"/>
+      <c r="E59" s="26" t="inlineStr">
         <is>
           <t>Being the amount paid to Lube Corner- Supply of consumble , Bill NO 1394:   Challan Number:   Manual PO [ CCEL Reno/PO/20245//8/87247(E)].  BA Team (A), Company Unit: Concrete Pole &amp; Pile, Project Name :  SPC Pole ( CCEL) Renovation. actual VN : 23011 in pole unit.</t>
         </is>
       </c>
-      <c r="F59" s="12" t="inlineStr"/>
-      <c r="G59" s="12" t="inlineStr"/>
-      <c r="H59" s="12" t="inlineStr"/>
-      <c r="I59" s="12" t="inlineStr"/>
-      <c r="J59" s="12" t="inlineStr"/>
-      <c r="K59" s="12" t="inlineStr"/>
-      <c r="L59" s="12" t="inlineStr">
+      <c r="F59" s="20" t="inlineStr"/>
+      <c r="G59" s="20" t="inlineStr"/>
+      <c r="H59" s="20" t="inlineStr"/>
+      <c r="I59" s="20" t="inlineStr"/>
+      <c r="J59" s="20" t="inlineStr"/>
+      <c r="K59" s="20" t="inlineStr"/>
+      <c r="L59" s="20" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="12" t="inlineStr">
+      <c r="A60" s="20" t="inlineStr">
         <is>
           <t>M004</t>
         </is>
       </c>
-      <c r="B60" s="13" t="inlineStr"/>
-      <c r="C60" s="12" t="inlineStr"/>
-      <c r="D60" s="12" t="inlineStr">
+      <c r="B60" s="21" t="inlineStr"/>
+      <c r="C60" s="20" t="inlineStr"/>
+      <c r="D60" s="20" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E60" s="19" t="inlineStr">
+      <c r="E60" s="27" t="inlineStr">
         <is>
           <t>nur.hossain</t>
         </is>
       </c>
-      <c r="F60" s="12" t="inlineStr"/>
-      <c r="G60" s="12" t="inlineStr"/>
-      <c r="H60" s="12" t="inlineStr"/>
-      <c r="I60" s="12" t="inlineStr"/>
-      <c r="J60" s="12" t="inlineStr"/>
-      <c r="K60" s="12" t="inlineStr"/>
-      <c r="L60" s="12" t="inlineStr">
+      <c r="F60" s="20" t="inlineStr"/>
+      <c r="G60" s="20" t="inlineStr"/>
+      <c r="H60" s="20" t="inlineStr"/>
+      <c r="I60" s="20" t="inlineStr"/>
+      <c r="J60" s="20" t="inlineStr"/>
+      <c r="K60" s="20" t="inlineStr"/>
+      <c r="L60" s="20" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="inlineStr"/>
-      <c r="B61" s="2" t="inlineStr"/>
-      <c r="C61" s="6" t="inlineStr">
+      <c r="A61" s="12" t="inlineStr">
+        <is>
+          <t>M127</t>
+        </is>
+      </c>
+      <c r="B61" s="13" t="inlineStr"/>
+      <c r="C61" s="14" t="inlineStr">
         <is>
           <t>05/Jun/2025</t>
         </is>
       </c>
-      <c r="D61" s="1" t="inlineStr">
+      <c r="D61" s="12" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E61" s="7" t="inlineStr">
+      <c r="E61" s="15" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F61" s="1" t="inlineStr"/>
-      <c r="G61" s="1" t="inlineStr"/>
-      <c r="H61" s="9" t="inlineStr">
+      <c r="F61" s="12" t="inlineStr"/>
+      <c r="G61" s="12" t="inlineStr"/>
+      <c r="H61" s="16" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I61" s="1" t="inlineStr">
+      <c r="I61" s="12" t="inlineStr">
         <is>
           <t>70846</t>
         </is>
       </c>
-      <c r="J61" s="8" t="inlineStr">
+      <c r="J61" s="17" t="inlineStr">
         <is>
           <t>20000</t>
         </is>
       </c>
-      <c r="K61" s="1" t="inlineStr"/>
-      <c r="L61" s="1" t="inlineStr"/>
+      <c r="K61" s="12" t="inlineStr"/>
+      <c r="L61" s="12" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="inlineStr"/>
-      <c r="B62" s="2" t="inlineStr">
-        <is>
-          <t>Unmatched Record
-Reasons:
-1. Amounts don't match: 20000 vs 10562.5
-2. Amounts don't match: 20000 vs 2700</t>
-        </is>
-      </c>
-      <c r="C62" s="1" t="inlineStr"/>
-      <c r="D62" s="1" t="inlineStr"/>
-      <c r="E62" s="10" t="inlineStr">
+      <c r="A62" s="12" t="inlineStr">
+        <is>
+          <t>M127</t>
+        </is>
+      </c>
+      <c r="B62" s="13" t="inlineStr">
+        <is>
+          <t>Manual Match
+Lender Amount: 20000.00
+Borrower Amount: 20000.00</t>
+        </is>
+      </c>
+      <c r="C62" s="12" t="inlineStr"/>
+      <c r="D62" s="12" t="inlineStr"/>
+      <c r="E62" s="18" t="inlineStr">
         <is>
           <t>Being the amount paid to-Chemitec -supply of consumble items , Bill NO 009:   Challan Number:   Manual PO [ CCEL Reno/PO/2024/8/87251)].  BA Team (A), Company Unit: Concrete Pole &amp; Pile, Project Name :  SPC Pole ( CCEL) Renovation. Actual VN:23018 in pole unite</t>
         </is>
       </c>
-      <c r="F62" s="1" t="inlineStr"/>
-      <c r="G62" s="1" t="inlineStr"/>
-      <c r="H62" s="1" t="inlineStr"/>
-      <c r="I62" s="1" t="inlineStr"/>
-      <c r="J62" s="1" t="inlineStr"/>
-      <c r="K62" s="1" t="inlineStr"/>
-      <c r="L62" s="1" t="inlineStr"/>
+      <c r="F62" s="12" t="inlineStr"/>
+      <c r="G62" s="12" t="inlineStr"/>
+      <c r="H62" s="12" t="inlineStr"/>
+      <c r="I62" s="12" t="inlineStr"/>
+      <c r="J62" s="12" t="inlineStr"/>
+      <c r="K62" s="12" t="inlineStr"/>
+      <c r="L62" s="12" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="inlineStr"/>
-      <c r="B63" s="2" t="inlineStr"/>
-      <c r="C63" s="1" t="inlineStr"/>
-      <c r="D63" s="1" t="inlineStr">
+      <c r="A63" s="12" t="inlineStr">
+        <is>
+          <t>M127</t>
+        </is>
+      </c>
+      <c r="B63" s="13" t="inlineStr"/>
+      <c r="C63" s="12" t="inlineStr"/>
+      <c r="D63" s="12" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E63" s="11" t="inlineStr">
+      <c r="E63" s="19" t="inlineStr">
         <is>
           <t>nur.hossain</t>
         </is>
       </c>
-      <c r="F63" s="1" t="inlineStr"/>
-      <c r="G63" s="1" t="inlineStr"/>
-      <c r="H63" s="1" t="inlineStr"/>
-      <c r="I63" s="1" t="inlineStr"/>
-      <c r="J63" s="1" t="inlineStr"/>
-      <c r="K63" s="1" t="inlineStr"/>
-      <c r="L63" s="1" t="inlineStr"/>
+      <c r="F63" s="12" t="inlineStr"/>
+      <c r="G63" s="12" t="inlineStr"/>
+      <c r="H63" s="12" t="inlineStr"/>
+      <c r="I63" s="12" t="inlineStr"/>
+      <c r="J63" s="12" t="inlineStr"/>
+      <c r="K63" s="12" t="inlineStr"/>
+      <c r="L63" s="12" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="inlineStr"/>
-      <c r="B64" s="2" t="inlineStr"/>
-      <c r="C64" s="6" t="inlineStr">
+      <c r="A64" s="20" t="inlineStr">
+        <is>
+          <t>M128</t>
+        </is>
+      </c>
+      <c r="B64" s="21" t="inlineStr"/>
+      <c r="C64" s="22" t="inlineStr">
         <is>
           <t>05/Jun/2025</t>
         </is>
       </c>
-      <c r="D64" s="1" t="inlineStr">
+      <c r="D64" s="20" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E64" s="7" t="inlineStr">
+      <c r="E64" s="23" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F64" s="1" t="inlineStr"/>
-      <c r="G64" s="1" t="inlineStr"/>
-      <c r="H64" s="9" t="inlineStr">
+      <c r="F64" s="20" t="inlineStr"/>
+      <c r="G64" s="20" t="inlineStr"/>
+      <c r="H64" s="24" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I64" s="1" t="inlineStr">
+      <c r="I64" s="20" t="inlineStr">
         <is>
           <t>70847</t>
         </is>
       </c>
-      <c r="J64" s="8" t="inlineStr">
+      <c r="J64" s="25" t="inlineStr">
         <is>
           <t>17500</t>
         </is>
       </c>
-      <c r="K64" s="1" t="inlineStr"/>
-      <c r="L64" s="1" t="inlineStr"/>
+      <c r="K64" s="20" t="inlineStr"/>
+      <c r="L64" s="20" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="inlineStr"/>
-      <c r="B65" s="2" t="inlineStr">
-        <is>
-          <t>Unmatched Record
-Reasons:
-1. Amounts don't match: 17500 vs 10562.5
-2. Amounts don't match: 17500 vs 2700</t>
-        </is>
-      </c>
-      <c r="C65" s="1" t="inlineStr"/>
-      <c r="D65" s="1" t="inlineStr"/>
-      <c r="E65" s="10" t="inlineStr">
+      <c r="A65" s="20" t="inlineStr">
+        <is>
+          <t>M128</t>
+        </is>
+      </c>
+      <c r="B65" s="21" t="inlineStr">
+        <is>
+          <t>Manual Match
+Lender Amount: 17500.00
+Borrower Amount: 17500.00</t>
+        </is>
+      </c>
+      <c r="C65" s="20" t="inlineStr"/>
+      <c r="D65" s="20" t="inlineStr"/>
+      <c r="E65" s="26" t="inlineStr">
         <is>
           <t>Being the amount -Safe Construction Solutions  to . against purchase CONSUMBLE ITEMS,    Challan Number:   Manual PO [ CCEL/Reno//PO///2024/9/21824-C] .bill no: 7951.  BA Team -Civil PEB unit. Company Unit: Concrete Pole &amp; Pile, Project Name :  SPC Pole ( CCEL) Renovation Actual VN: 23042 in pole unit</t>
         </is>
       </c>
-      <c r="F65" s="1" t="inlineStr"/>
-      <c r="G65" s="1" t="inlineStr"/>
-      <c r="H65" s="1" t="inlineStr"/>
-      <c r="I65" s="1" t="inlineStr"/>
-      <c r="J65" s="1" t="inlineStr"/>
-      <c r="K65" s="1" t="inlineStr"/>
-      <c r="L65" s="1" t="inlineStr"/>
+      <c r="F65" s="20" t="inlineStr"/>
+      <c r="G65" s="20" t="inlineStr"/>
+      <c r="H65" s="20" t="inlineStr"/>
+      <c r="I65" s="20" t="inlineStr"/>
+      <c r="J65" s="20" t="inlineStr"/>
+      <c r="K65" s="20" t="inlineStr"/>
+      <c r="L65" s="20" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="inlineStr"/>
-      <c r="B66" s="2" t="inlineStr"/>
-      <c r="C66" s="1" t="inlineStr"/>
-      <c r="D66" s="1" t="inlineStr">
+      <c r="A66" s="20" t="inlineStr">
+        <is>
+          <t>M128</t>
+        </is>
+      </c>
+      <c r="B66" s="21" t="inlineStr"/>
+      <c r="C66" s="20" t="inlineStr"/>
+      <c r="D66" s="20" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E66" s="11" t="inlineStr">
+      <c r="E66" s="27" t="inlineStr">
         <is>
           <t>nur.hossain</t>
         </is>
       </c>
-      <c r="F66" s="1" t="inlineStr"/>
-      <c r="G66" s="1" t="inlineStr"/>
-      <c r="H66" s="1" t="inlineStr"/>
-      <c r="I66" s="1" t="inlineStr"/>
-      <c r="J66" s="1" t="inlineStr"/>
-      <c r="K66" s="1" t="inlineStr"/>
-      <c r="L66" s="1" t="inlineStr"/>
+      <c r="F66" s="20" t="inlineStr"/>
+      <c r="G66" s="20" t="inlineStr"/>
+      <c r="H66" s="20" t="inlineStr"/>
+      <c r="I66" s="20" t="inlineStr"/>
+      <c r="J66" s="20" t="inlineStr"/>
+      <c r="K66" s="20" t="inlineStr"/>
+      <c r="L66" s="20" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="inlineStr"/>
-      <c r="B67" s="2" t="inlineStr"/>
-      <c r="C67" s="6" t="inlineStr">
+      <c r="A67" s="12" t="inlineStr">
+        <is>
+          <t>M129</t>
+        </is>
+      </c>
+      <c r="B67" s="13" t="inlineStr"/>
+      <c r="C67" s="14" t="inlineStr">
         <is>
           <t>05/Jun/2025</t>
         </is>
       </c>
-      <c r="D67" s="1" t="inlineStr">
+      <c r="D67" s="12" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E67" s="7" t="inlineStr">
+      <c r="E67" s="15" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F67" s="1" t="inlineStr"/>
-      <c r="G67" s="1" t="inlineStr"/>
-      <c r="H67" s="9" t="inlineStr">
+      <c r="F67" s="12" t="inlineStr"/>
+      <c r="G67" s="12" t="inlineStr"/>
+      <c r="H67" s="16" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I67" s="1" t="inlineStr">
+      <c r="I67" s="12" t="inlineStr">
         <is>
           <t>70848</t>
         </is>
       </c>
-      <c r="J67" s="8" t="inlineStr">
+      <c r="J67" s="17" t="inlineStr">
         <is>
           <t>110839</t>
         </is>
       </c>
-      <c r="K67" s="1" t="inlineStr"/>
-      <c r="L67" s="1" t="inlineStr"/>
+      <c r="K67" s="12" t="inlineStr"/>
+      <c r="L67" s="12" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="inlineStr"/>
-      <c r="B68" s="2" t="inlineStr">
-        <is>
-          <t>Unmatched Record
-Reasons:
-1. Amounts don't match: 110839 vs 10562.5
-2. Amounts don't match: 110839 vs 2700</t>
-        </is>
-      </c>
-      <c r="C68" s="1" t="inlineStr"/>
-      <c r="D68" s="1" t="inlineStr"/>
-      <c r="E68" s="10" t="inlineStr">
+      <c r="A68" s="12" t="inlineStr">
+        <is>
+          <t>M129</t>
+        </is>
+      </c>
+      <c r="B68" s="13" t="inlineStr">
+        <is>
+          <t>Manual Match
+Lender Amount: 110839.00
+Borrower Amount: 110839.00</t>
+        </is>
+      </c>
+      <c r="C68" s="12" t="inlineStr"/>
+      <c r="D68" s="12" t="inlineStr"/>
+      <c r="E68" s="18" t="inlineStr">
         <is>
           <t>Being the amount paid to Pragati Life Insurance Limited agt. Group Insurance Renewal Bill. Bill No.: 00633 &amp; 00633-C. Bill period: 1 march -2025 to 28 feb -2026</t>
         </is>
       </c>
-      <c r="F68" s="1" t="inlineStr"/>
-      <c r="G68" s="1" t="inlineStr"/>
-      <c r="H68" s="1" t="inlineStr"/>
-      <c r="I68" s="1" t="inlineStr"/>
-      <c r="J68" s="1" t="inlineStr"/>
-      <c r="K68" s="1" t="inlineStr"/>
-      <c r="L68" s="1" t="inlineStr"/>
+      <c r="F68" s="12" t="inlineStr"/>
+      <c r="G68" s="12" t="inlineStr"/>
+      <c r="H68" s="12" t="inlineStr"/>
+      <c r="I68" s="12" t="inlineStr"/>
+      <c r="J68" s="12" t="inlineStr"/>
+      <c r="K68" s="12" t="inlineStr"/>
+      <c r="L68" s="12" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="inlineStr"/>
-      <c r="B69" s="2" t="inlineStr"/>
-      <c r="C69" s="1" t="inlineStr"/>
-      <c r="D69" s="1" t="inlineStr">
+      <c r="A69" s="12" t="inlineStr">
+        <is>
+          <t>M129</t>
+        </is>
+      </c>
+      <c r="B69" s="13" t="inlineStr"/>
+      <c r="C69" s="12" t="inlineStr"/>
+      <c r="D69" s="12" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E69" s="11" t="inlineStr">
+      <c r="E69" s="19" t="inlineStr">
         <is>
           <t>nur.hossain</t>
         </is>
       </c>
-      <c r="F69" s="1" t="inlineStr"/>
-      <c r="G69" s="1" t="inlineStr"/>
-      <c r="H69" s="1" t="inlineStr"/>
-      <c r="I69" s="1" t="inlineStr"/>
-      <c r="J69" s="1" t="inlineStr"/>
-      <c r="K69" s="1" t="inlineStr"/>
-      <c r="L69" s="1" t="inlineStr"/>
+      <c r="F69" s="12" t="inlineStr"/>
+      <c r="G69" s="12" t="inlineStr"/>
+      <c r="H69" s="12" t="inlineStr"/>
+      <c r="I69" s="12" t="inlineStr"/>
+      <c r="J69" s="12" t="inlineStr"/>
+      <c r="K69" s="12" t="inlineStr"/>
+      <c r="L69" s="12" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="20" t="inlineStr">
@@ -8242,516 +8334,540 @@
       </c>
     </row>
     <row r="221">
-      <c r="A221" s="1" t="inlineStr"/>
-      <c r="B221" s="2" t="inlineStr"/>
-      <c r="C221" s="6" t="inlineStr">
+      <c r="A221" s="20" t="inlineStr">
+        <is>
+          <t>M130</t>
+        </is>
+      </c>
+      <c r="B221" s="21" t="inlineStr"/>
+      <c r="C221" s="22" t="inlineStr">
         <is>
           <t>23/Jun/2025</t>
         </is>
       </c>
-      <c r="D221" s="1" t="inlineStr">
+      <c r="D221" s="20" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E221" s="7" t="inlineStr">
+      <c r="E221" s="23" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F221" s="1" t="inlineStr"/>
-      <c r="G221" s="1" t="inlineStr"/>
-      <c r="H221" s="9" t="inlineStr">
+      <c r="F221" s="20" t="inlineStr"/>
+      <c r="G221" s="20" t="inlineStr"/>
+      <c r="H221" s="24" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I221" s="1" t="inlineStr">
+      <c r="I221" s="20" t="inlineStr">
         <is>
           <t>70568</t>
         </is>
       </c>
-      <c r="J221" s="8" t="inlineStr">
+      <c r="J221" s="25" t="inlineStr">
         <is>
           <t>24000000</t>
         </is>
       </c>
-      <c r="K221" s="1" t="inlineStr"/>
-      <c r="L221" s="1" t="inlineStr"/>
+      <c r="K221" s="20" t="inlineStr"/>
+      <c r="L221" s="20" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="222">
-      <c r="A222" s="1" t="inlineStr"/>
-      <c r="B222" s="2" t="inlineStr">
-        <is>
-          <t>Unmatched Record
-Reasons:
-1. Borrower's narration does not contain lender's short code</t>
-        </is>
-      </c>
-      <c r="C222" s="1" t="inlineStr"/>
-      <c r="D222" s="1" t="inlineStr"/>
-      <c r="E222" s="10" t="inlineStr">
+      <c r="A222" s="20" t="inlineStr">
+        <is>
+          <t>M130</t>
+        </is>
+      </c>
+      <c r="B222" s="21" t="inlineStr">
+        <is>
+          <t>Manual Match
+Lender Amount: 24000000.00
+Borrower Amount: 24000000.00</t>
+        </is>
+      </c>
+      <c r="C222" s="20" t="inlineStr"/>
+      <c r="D222" s="20" t="inlineStr"/>
+      <c r="E222" s="26" t="inlineStr">
         <is>
           <t>Interunit fund Transfer as Inter Unit Loan A/C-Pole Unit, MDBL#00304</t>
         </is>
       </c>
-      <c r="F222" s="1" t="inlineStr"/>
-      <c r="G222" s="1" t="inlineStr"/>
-      <c r="H222" s="1" t="inlineStr"/>
-      <c r="I222" s="1" t="inlineStr"/>
-      <c r="J222" s="1" t="inlineStr"/>
-      <c r="K222" s="1" t="inlineStr"/>
-      <c r="L222" s="1" t="inlineStr"/>
+      <c r="F222" s="20" t="inlineStr"/>
+      <c r="G222" s="20" t="inlineStr"/>
+      <c r="H222" s="20" t="inlineStr"/>
+      <c r="I222" s="20" t="inlineStr"/>
+      <c r="J222" s="20" t="inlineStr"/>
+      <c r="K222" s="20" t="inlineStr"/>
+      <c r="L222" s="20" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="223">
-      <c r="A223" s="1" t="inlineStr"/>
-      <c r="B223" s="2" t="inlineStr"/>
-      <c r="C223" s="1" t="inlineStr"/>
-      <c r="D223" s="1" t="inlineStr">
+      <c r="A223" s="20" t="inlineStr">
+        <is>
+          <t>M130</t>
+        </is>
+      </c>
+      <c r="B223" s="21" t="inlineStr"/>
+      <c r="C223" s="20" t="inlineStr"/>
+      <c r="D223" s="20" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E223" s="11" t="inlineStr">
+      <c r="E223" s="27" t="inlineStr">
         <is>
           <t>ashiq</t>
         </is>
       </c>
-      <c r="F223" s="1" t="inlineStr"/>
-      <c r="G223" s="1" t="inlineStr"/>
-      <c r="H223" s="1" t="inlineStr"/>
-      <c r="I223" s="1" t="inlineStr"/>
-      <c r="J223" s="1" t="inlineStr"/>
-      <c r="K223" s="1" t="inlineStr"/>
-      <c r="L223" s="1" t="inlineStr"/>
+      <c r="F223" s="20" t="inlineStr"/>
+      <c r="G223" s="20" t="inlineStr"/>
+      <c r="H223" s="20" t="inlineStr"/>
+      <c r="I223" s="20" t="inlineStr"/>
+      <c r="J223" s="20" t="inlineStr"/>
+      <c r="K223" s="20" t="inlineStr"/>
+      <c r="L223" s="20" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
     </row>
     <row r="224">
-      <c r="A224" s="20" t="inlineStr">
+      <c r="A224" s="12" t="inlineStr">
         <is>
           <t>M061</t>
         </is>
       </c>
-      <c r="B224" s="21" t="inlineStr"/>
-      <c r="C224" s="22" t="inlineStr">
+      <c r="B224" s="13" t="inlineStr"/>
+      <c r="C224" s="14" t="inlineStr">
         <is>
           <t>24/Jun/2025</t>
         </is>
       </c>
-      <c r="D224" s="20" t="inlineStr">
+      <c r="D224" s="12" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E224" s="23" t="inlineStr">
+      <c r="E224" s="15" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F224" s="20" t="inlineStr"/>
-      <c r="G224" s="20" t="inlineStr"/>
-      <c r="H224" s="24" t="inlineStr">
+      <c r="F224" s="12" t="inlineStr"/>
+      <c r="G224" s="12" t="inlineStr"/>
+      <c r="H224" s="16" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I224" s="20" t="inlineStr">
+      <c r="I224" s="12" t="inlineStr">
         <is>
           <t>70572</t>
         </is>
       </c>
-      <c r="J224" s="25" t="inlineStr">
+      <c r="J224" s="17" t="inlineStr">
         <is>
           <t>1235000</t>
         </is>
       </c>
-      <c r="K224" s="20" t="inlineStr"/>
-      <c r="L224" s="20" t="inlineStr">
+      <c r="K224" s="12" t="inlineStr"/>
+      <c r="L224" s="12" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="225">
-      <c r="A225" s="20" t="inlineStr">
+      <c r="A225" s="12" t="inlineStr">
         <is>
           <t>M061</t>
         </is>
       </c>
-      <c r="B225" s="21" t="inlineStr">
+      <c r="B225" s="13" t="inlineStr">
         <is>
           <t>LC Match: LC-187724010094/24
 Lender Amount: 1235000.00
 Borrower Amount: 1235000.00</t>
         </is>
       </c>
-      <c r="C225" s="20" t="inlineStr"/>
-      <c r="D225" s="20" t="inlineStr"/>
-      <c r="E225" s="26" t="inlineStr">
+      <c r="C225" s="12" t="inlineStr"/>
+      <c r="D225" s="12" t="inlineStr"/>
+      <c r="E225" s="18" t="inlineStr">
         <is>
           <t>Amount being paid as Port,Shipping &amp; Carrying charges agt LC-187724010094/24[Item-11,000 MT Crushed Stone-Project-G-24-Lot-1-Team-A]</t>
         </is>
       </c>
-      <c r="F225" s="20" t="inlineStr"/>
-      <c r="G225" s="20" t="inlineStr"/>
-      <c r="H225" s="20" t="inlineStr"/>
-      <c r="I225" s="20" t="inlineStr"/>
-      <c r="J225" s="20" t="inlineStr"/>
-      <c r="K225" s="20" t="inlineStr"/>
-      <c r="L225" s="20" t="inlineStr">
+      <c r="F225" s="12" t="inlineStr"/>
+      <c r="G225" s="12" t="inlineStr"/>
+      <c r="H225" s="12" t="inlineStr"/>
+      <c r="I225" s="12" t="inlineStr"/>
+      <c r="J225" s="12" t="inlineStr"/>
+      <c r="K225" s="12" t="inlineStr"/>
+      <c r="L225" s="12" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="226">
-      <c r="A226" s="20" t="inlineStr">
+      <c r="A226" s="12" t="inlineStr">
         <is>
           <t>M061</t>
         </is>
       </c>
-      <c r="B226" s="21" t="inlineStr"/>
-      <c r="C226" s="20" t="inlineStr"/>
-      <c r="D226" s="20" t="inlineStr">
+      <c r="B226" s="13" t="inlineStr"/>
+      <c r="C226" s="12" t="inlineStr"/>
+      <c r="D226" s="12" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E226" s="27" t="inlineStr">
+      <c r="E226" s="19" t="inlineStr">
         <is>
           <t>shabbirul</t>
         </is>
       </c>
-      <c r="F226" s="20" t="inlineStr"/>
-      <c r="G226" s="20" t="inlineStr"/>
-      <c r="H226" s="20" t="inlineStr"/>
-      <c r="I226" s="20" t="inlineStr"/>
-      <c r="J226" s="20" t="inlineStr"/>
-      <c r="K226" s="20" t="inlineStr"/>
-      <c r="L226" s="20" t="inlineStr">
+      <c r="F226" s="12" t="inlineStr"/>
+      <c r="G226" s="12" t="inlineStr"/>
+      <c r="H226" s="12" t="inlineStr"/>
+      <c r="I226" s="12" t="inlineStr"/>
+      <c r="J226" s="12" t="inlineStr"/>
+      <c r="K226" s="12" t="inlineStr"/>
+      <c r="L226" s="12" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="227">
-      <c r="A227" s="12" t="inlineStr">
+      <c r="A227" s="20" t="inlineStr">
         <is>
           <t>M121</t>
         </is>
       </c>
-      <c r="B227" s="13" t="inlineStr"/>
-      <c r="C227" s="14" t="inlineStr">
+      <c r="B227" s="21" t="inlineStr"/>
+      <c r="C227" s="22" t="inlineStr">
         <is>
           <t>25/Jun/2025</t>
         </is>
       </c>
-      <c r="D227" s="12" t="inlineStr">
+      <c r="D227" s="20" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E227" s="15" t="inlineStr">
+      <c r="E227" s="23" t="inlineStr">
         <is>
           <t>Eastern Bank,STD-1011220144056</t>
         </is>
       </c>
-      <c r="F227" s="12" t="inlineStr"/>
-      <c r="G227" s="12" t="inlineStr"/>
-      <c r="H227" s="16" t="inlineStr">
+      <c r="F227" s="20" t="inlineStr"/>
+      <c r="G227" s="20" t="inlineStr"/>
+      <c r="H227" s="24" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I227" s="12" t="inlineStr">
+      <c r="I227" s="20" t="inlineStr">
         <is>
           <t>70556</t>
         </is>
       </c>
-      <c r="J227" s="17" t="inlineStr">
+      <c r="J227" s="25" t="inlineStr">
         <is>
           <t>1300000</t>
         </is>
       </c>
-      <c r="K227" s="12" t="inlineStr"/>
-      <c r="L227" s="12" t="inlineStr">
+      <c r="K227" s="20" t="inlineStr"/>
+      <c r="L227" s="20" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="228">
-      <c r="A228" s="12" t="inlineStr">
+      <c r="A228" s="20" t="inlineStr">
         <is>
           <t>M121</t>
         </is>
       </c>
-      <c r="B228" s="13" t="inlineStr">
+      <c r="B228" s="21" t="inlineStr">
         <is>
           <t>Interunit Loan Match: EBL#4056
 Lender Amount: 1300000.00
 Borrower Amount: 1300000.00</t>
         </is>
       </c>
-      <c r="C228" s="12" t="inlineStr"/>
-      <c r="D228" s="12" t="inlineStr"/>
-      <c r="E228" s="18" t="inlineStr">
+      <c r="C228" s="20" t="inlineStr"/>
+      <c r="D228" s="20" t="inlineStr"/>
+      <c r="E228" s="26" t="inlineStr">
         <is>
           <t>Interunit fund transfer as Inter Unit Loan A/C-Pole Unit,EBL#44056</t>
         </is>
       </c>
-      <c r="F228" s="12" t="inlineStr"/>
-      <c r="G228" s="12" t="inlineStr"/>
-      <c r="H228" s="12" t="inlineStr"/>
-      <c r="I228" s="12" t="inlineStr"/>
-      <c r="J228" s="12" t="inlineStr"/>
-      <c r="K228" s="12" t="inlineStr"/>
-      <c r="L228" s="12" t="inlineStr">
+      <c r="F228" s="20" t="inlineStr"/>
+      <c r="G228" s="20" t="inlineStr"/>
+      <c r="H228" s="20" t="inlineStr"/>
+      <c r="I228" s="20" t="inlineStr"/>
+      <c r="J228" s="20" t="inlineStr"/>
+      <c r="K228" s="20" t="inlineStr"/>
+      <c r="L228" s="20" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="229">
-      <c r="A229" s="12" t="inlineStr">
+      <c r="A229" s="20" t="inlineStr">
         <is>
           <t>M121</t>
         </is>
       </c>
-      <c r="B229" s="13" t="inlineStr"/>
-      <c r="C229" s="12" t="inlineStr"/>
-      <c r="D229" s="12" t="inlineStr">
+      <c r="B229" s="21" t="inlineStr"/>
+      <c r="C229" s="20" t="inlineStr"/>
+      <c r="D229" s="20" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E229" s="19" t="inlineStr">
+      <c r="E229" s="27" t="inlineStr">
         <is>
           <t>ashiq</t>
         </is>
       </c>
-      <c r="F229" s="12" t="inlineStr"/>
-      <c r="G229" s="12" t="inlineStr"/>
-      <c r="H229" s="12" t="inlineStr"/>
-      <c r="I229" s="12" t="inlineStr"/>
-      <c r="J229" s="12" t="inlineStr"/>
-      <c r="K229" s="12" t="inlineStr"/>
-      <c r="L229" s="12" t="inlineStr">
+      <c r="F229" s="20" t="inlineStr"/>
+      <c r="G229" s="20" t="inlineStr"/>
+      <c r="H229" s="20" t="inlineStr"/>
+      <c r="I229" s="20" t="inlineStr"/>
+      <c r="J229" s="20" t="inlineStr"/>
+      <c r="K229" s="20" t="inlineStr"/>
+      <c r="L229" s="20" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="230">
-      <c r="A230" s="20" t="inlineStr">
+      <c r="A230" s="12" t="inlineStr">
         <is>
           <t>M063</t>
         </is>
       </c>
-      <c r="B230" s="21" t="inlineStr"/>
-      <c r="C230" s="22" t="inlineStr">
+      <c r="B230" s="13" t="inlineStr"/>
+      <c r="C230" s="14" t="inlineStr">
         <is>
           <t>26/Jun/2025</t>
         </is>
       </c>
-      <c r="D230" s="20" t="inlineStr">
+      <c r="D230" s="12" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E230" s="23" t="inlineStr">
+      <c r="E230" s="15" t="inlineStr">
         <is>
           <t>Prime Bank-CD-2126117010855</t>
         </is>
       </c>
-      <c r="F230" s="20" t="inlineStr"/>
-      <c r="G230" s="20" t="inlineStr"/>
-      <c r="H230" s="24" t="inlineStr">
+      <c r="F230" s="12" t="inlineStr"/>
+      <c r="G230" s="12" t="inlineStr"/>
+      <c r="H230" s="16" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I230" s="20" t="inlineStr">
+      <c r="I230" s="12" t="inlineStr">
         <is>
           <t>3188</t>
         </is>
       </c>
-      <c r="J230" s="25" t="inlineStr">
+      <c r="J230" s="17" t="inlineStr">
         <is>
           <t>43496089</t>
         </is>
       </c>
-      <c r="K230" s="20" t="inlineStr"/>
-      <c r="L230" s="20" t="inlineStr">
+      <c r="K230" s="12" t="inlineStr"/>
+      <c r="L230" s="12" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="231">
-      <c r="A231" s="20" t="inlineStr">
+      <c r="A231" s="12" t="inlineStr">
         <is>
           <t>M063</t>
         </is>
       </c>
-      <c r="B231" s="21" t="inlineStr">
+      <c r="B231" s="13" t="inlineStr">
         <is>
           <t>USD Match: $.789,663.20
 Lender Amount: 43496089.00
 Borrower Amount: 43496089.00</t>
         </is>
       </c>
-      <c r="C231" s="20" t="inlineStr"/>
-      <c r="D231" s="20" t="inlineStr"/>
-      <c r="E231" s="26" t="inlineStr">
+      <c r="C231" s="12" t="inlineStr"/>
+      <c r="D231" s="12" t="inlineStr"/>
+      <c r="E231" s="18" t="inlineStr">
         <is>
           <t>Amount paid agst Contract no.MCEP/BREB/DMD-SPC-G-24-Lot-1/2023-2024. Date.07.07.2024 This amount actually Pole Unit but deposit in Geo Textile Unit. Total bill amount $.789,663.20/- But ($.443,663.42+$6,400) Deposit in Geo Textile Unit. Remaining   $339520.78 Deposit in Steel Unit. Bank charge-$80. Rate.122.60, Total Received amount $.789583.20, Deposit amount JV partner Vicar Concrete Products $363,103.21 Remaing amount deposit in CIL.</t>
         </is>
       </c>
-      <c r="F231" s="20" t="inlineStr"/>
-      <c r="G231" s="20" t="inlineStr"/>
-      <c r="H231" s="20" t="inlineStr"/>
-      <c r="I231" s="20" t="inlineStr"/>
-      <c r="J231" s="20" t="inlineStr"/>
-      <c r="K231" s="20" t="inlineStr"/>
-      <c r="L231" s="20" t="inlineStr">
+      <c r="F231" s="12" t="inlineStr"/>
+      <c r="G231" s="12" t="inlineStr"/>
+      <c r="H231" s="12" t="inlineStr"/>
+      <c r="I231" s="12" t="inlineStr"/>
+      <c r="J231" s="12" t="inlineStr"/>
+      <c r="K231" s="12" t="inlineStr"/>
+      <c r="L231" s="12" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="232">
-      <c r="A232" s="20" t="inlineStr">
+      <c r="A232" s="12" t="inlineStr">
         <is>
           <t>M063</t>
         </is>
       </c>
-      <c r="B232" s="21" t="inlineStr"/>
-      <c r="C232" s="20" t="inlineStr"/>
-      <c r="D232" s="20" t="inlineStr">
+      <c r="B232" s="13" t="inlineStr"/>
+      <c r="C232" s="12" t="inlineStr"/>
+      <c r="D232" s="12" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E232" s="27" t="inlineStr">
+      <c r="E232" s="19" t="inlineStr">
         <is>
           <t>ashiq</t>
         </is>
       </c>
-      <c r="F232" s="20" t="inlineStr"/>
-      <c r="G232" s="20" t="inlineStr"/>
-      <c r="H232" s="20" t="inlineStr"/>
-      <c r="I232" s="20" t="inlineStr"/>
-      <c r="J232" s="20" t="inlineStr"/>
-      <c r="K232" s="20" t="inlineStr"/>
-      <c r="L232" s="20" t="inlineStr">
+      <c r="F232" s="12" t="inlineStr"/>
+      <c r="G232" s="12" t="inlineStr"/>
+      <c r="H232" s="12" t="inlineStr"/>
+      <c r="I232" s="12" t="inlineStr"/>
+      <c r="J232" s="12" t="inlineStr"/>
+      <c r="K232" s="12" t="inlineStr"/>
+      <c r="L232" s="12" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="233">
-      <c r="A233" s="12" t="inlineStr">
+      <c r="A233" s="20" t="inlineStr">
         <is>
           <t>M065</t>
         </is>
       </c>
-      <c r="B233" s="13" t="inlineStr"/>
-      <c r="C233" s="14" t="inlineStr">
+      <c r="B233" s="21" t="inlineStr"/>
+      <c r="C233" s="22" t="inlineStr">
         <is>
           <t>30/Jun/2025</t>
         </is>
       </c>
-      <c r="D233" s="12" t="inlineStr">
+      <c r="D233" s="20" t="inlineStr">
         <is>
           <t>Dr</t>
         </is>
       </c>
-      <c r="E233" s="15" t="inlineStr">
+      <c r="E233" s="23" t="inlineStr">
         <is>
           <t>Salary &amp; Allowance Payable</t>
         </is>
       </c>
-      <c r="F233" s="12" t="inlineStr"/>
-      <c r="G233" s="12" t="inlineStr"/>
-      <c r="H233" s="16" t="inlineStr">
+      <c r="F233" s="20" t="inlineStr"/>
+      <c r="G233" s="20" t="inlineStr"/>
+      <c r="H233" s="24" t="inlineStr">
         <is>
           <t>Journal</t>
         </is>
       </c>
-      <c r="I233" s="12" t="inlineStr">
+      <c r="I233" s="20" t="inlineStr">
         <is>
           <t>3855</t>
         </is>
       </c>
-      <c r="J233" s="12" t="inlineStr"/>
-      <c r="K233" s="17" t="inlineStr">
+      <c r="J233" s="20" t="inlineStr"/>
+      <c r="K233" s="25" t="inlineStr">
         <is>
           <t>20733</t>
         </is>
       </c>
-      <c r="L233" s="12" t="inlineStr">
+      <c r="L233" s="20" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="234">
-      <c r="A234" s="12" t="inlineStr">
+      <c r="A234" s="20" t="inlineStr">
         <is>
           <t>M065</t>
         </is>
       </c>
-      <c r="B234" s="13" t="inlineStr">
+      <c r="B234" s="21" t="inlineStr">
         <is>
           <t>Narration Match
 Lender Amount: 20733.00
 Borrower Amount: 20733.00</t>
         </is>
       </c>
-      <c r="C234" s="12" t="inlineStr"/>
-      <c r="D234" s="12" t="inlineStr"/>
-      <c r="E234" s="18" t="inlineStr">
+      <c r="C234" s="20" t="inlineStr"/>
+      <c r="D234" s="20" t="inlineStr"/>
+      <c r="E234" s="26" t="inlineStr">
         <is>
           <t>Salary of Pole unit paid to Steel unit for the month of June-2025.</t>
         </is>
       </c>
-      <c r="F234" s="12" t="inlineStr"/>
-      <c r="G234" s="12" t="inlineStr"/>
-      <c r="H234" s="12" t="inlineStr"/>
-      <c r="I234" s="12" t="inlineStr"/>
-      <c r="J234" s="12" t="inlineStr"/>
-      <c r="K234" s="12" t="inlineStr"/>
-      <c r="L234" s="12" t="inlineStr">
+      <c r="F234" s="20" t="inlineStr"/>
+      <c r="G234" s="20" t="inlineStr"/>
+      <c r="H234" s="20" t="inlineStr"/>
+      <c r="I234" s="20" t="inlineStr"/>
+      <c r="J234" s="20" t="inlineStr"/>
+      <c r="K234" s="20" t="inlineStr"/>
+      <c r="L234" s="20" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="235">
-      <c r="A235" s="12" t="inlineStr">
+      <c r="A235" s="20" t="inlineStr">
         <is>
           <t>M065</t>
         </is>
       </c>
-      <c r="B235" s="13" t="inlineStr"/>
-      <c r="C235" s="12" t="inlineStr"/>
-      <c r="D235" s="12" t="inlineStr">
+      <c r="B235" s="21" t="inlineStr"/>
+      <c r="C235" s="20" t="inlineStr"/>
+      <c r="D235" s="20" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E235" s="19" t="inlineStr">
+      <c r="E235" s="27" t="inlineStr">
         <is>
           <t>sayeda</t>
         </is>
       </c>
-      <c r="F235" s="12" t="inlineStr"/>
-      <c r="G235" s="12" t="inlineStr"/>
-      <c r="H235" s="12" t="inlineStr"/>
-      <c r="I235" s="12" t="inlineStr"/>
-      <c r="J235" s="12" t="inlineStr"/>
-      <c r="K235" s="12" t="inlineStr"/>
-      <c r="L235" s="12" t="inlineStr">
+      <c r="F235" s="20" t="inlineStr"/>
+      <c r="G235" s="20" t="inlineStr"/>
+      <c r="H235" s="20" t="inlineStr"/>
+      <c r="I235" s="20" t="inlineStr"/>
+      <c r="J235" s="20" t="inlineStr"/>
+      <c r="K235" s="20" t="inlineStr"/>
+      <c r="L235" s="20" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>

</xml_diff>